<commit_message>
Ajout des fichiers de rapports dans .gitignore
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbenjemi\Katalon Studio\ANEF_Eloignement_V1_Nawres\ANEF-Eloignement\ANEF_Eloignement_V1_Nawres\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAF2BAB-2A55-466B-9AE6-A93DC5BDFD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F348A98-BB3D-4582-94F5-22146F8EA5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JDD" sheetId="6" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="688">
   <si>
     <t>URL_ANEFdevfenv5</t>
   </si>
@@ -2102,6 +2102,15 @@
   </si>
   <si>
     <t>AjouterIRTF2</t>
+  </si>
+  <si>
+    <t>FondementLegalVisite</t>
+  </si>
+  <si>
+    <t>FondementAssignationResidence</t>
+  </si>
+  <si>
+    <t>ReexamenExpulsion</t>
   </si>
 </sst>
 </file>
@@ -2938,15 +2947,78 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2957,69 +3029,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3336,10 +3345,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}">
   <dimension ref="A1:FQ173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AH1" sqref="AH1"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3535,9 +3544,15 @@
       <c r="AN1" s="24" t="s">
         <v>684</v>
       </c>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="14"/>
+      <c r="AO1" s="24" t="s">
+        <v>685</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>686</v>
+      </c>
+      <c r="AQ1" s="14" t="s">
+        <v>687</v>
+      </c>
       <c r="AR1" s="13"/>
       <c r="AS1" s="13"/>
       <c r="AT1" s="24"/>
@@ -3681,7 +3696,7 @@
         <v>658</v>
       </c>
       <c r="E2" s="107" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F2" s="107">
         <v>7503182107</v>
@@ -7131,12 +7146,12 @@
       <c r="AF20" s="38"/>
     </row>
     <row r="21" spans="1:170" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="140" t="s">
+      <c r="A21" s="122" t="s">
         <v>600</v>
       </c>
-      <c r="B21" s="141"/>
-      <c r="C21" s="141"/>
-      <c r="D21" s="141"/>
+      <c r="B21" s="123"/>
+      <c r="C21" s="123"/>
+      <c r="D21" s="123"/>
       <c r="E21" s="82"/>
       <c r="F21" s="82"/>
       <c r="G21" s="82"/>
@@ -7158,350 +7173,350 @@
       <c r="W21" s="82"/>
     </row>
     <row r="22" spans="1:170" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="142" t="s">
+      <c r="A22" s="124" t="s">
         <v>601</v>
       </c>
-      <c r="B22" s="142"/>
+      <c r="B22" s="124"/>
       <c r="C22" s="86" t="s">
         <v>602</v>
       </c>
-      <c r="D22" s="146"/>
+      <c r="D22" s="131"/>
     </row>
     <row r="23" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A23" s="143" t="s">
+      <c r="A23" s="125" t="s">
         <v>218</v>
       </c>
-      <c r="B23" s="144"/>
+      <c r="B23" s="126"/>
       <c r="C23" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="146"/>
+      <c r="D23" s="131"/>
     </row>
     <row r="24" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A24" s="121" t="s">
+      <c r="A24" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="126"/>
+      <c r="B24" s="128"/>
       <c r="C24" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="146"/>
+      <c r="D24" s="131"/>
     </row>
     <row r="25" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A25" s="121"/>
-      <c r="B25" s="126"/>
+      <c r="A25" s="127"/>
+      <c r="B25" s="128"/>
       <c r="C25" s="83" t="s">
         <v>599</v>
       </c>
-      <c r="D25" s="146"/>
+      <c r="D25" s="131"/>
     </row>
     <row r="26" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A26" s="136" t="s">
+      <c r="A26" s="129" t="s">
         <v>603</v>
       </c>
-      <c r="B26" s="145"/>
+      <c r="B26" s="130"/>
       <c r="C26" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="146"/>
+      <c r="D26" s="131"/>
     </row>
     <row r="27" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A27" s="136"/>
-      <c r="B27" s="145"/>
+      <c r="A27" s="129"/>
+      <c r="B27" s="130"/>
       <c r="C27" s="84" t="s">
         <v>604</v>
       </c>
-      <c r="D27" s="146"/>
+      <c r="D27" s="131"/>
     </row>
     <row r="28" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A28" s="121" t="s">
+      <c r="A28" s="127" t="s">
         <v>605</v>
       </c>
-      <c r="B28" s="126"/>
+      <c r="B28" s="128"/>
       <c r="C28" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="146"/>
+      <c r="D28" s="131"/>
     </row>
     <row r="29" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A29" s="121"/>
-      <c r="B29" s="126"/>
+      <c r="A29" s="127"/>
+      <c r="B29" s="128"/>
       <c r="C29" s="83" t="s">
         <v>606</v>
       </c>
-      <c r="D29" s="146"/>
+      <c r="D29" s="131"/>
     </row>
     <row r="30" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A30" s="136" t="s">
+      <c r="A30" s="129" t="s">
         <v>607</v>
       </c>
-      <c r="B30" s="136"/>
+      <c r="B30" s="129"/>
       <c r="C30" s="84" t="s">
         <v>608</v>
       </c>
-      <c r="D30" s="146"/>
+      <c r="D30" s="131"/>
     </row>
     <row r="31" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A31" s="136"/>
-      <c r="B31" s="136"/>
+      <c r="A31" s="129"/>
+      <c r="B31" s="129"/>
       <c r="C31" s="84" t="s">
         <v>609</v>
       </c>
-      <c r="D31" s="146"/>
+      <c r="D31" s="131"/>
     </row>
     <row r="32" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A32" s="138" t="s">
+      <c r="A32" s="133" t="s">
         <v>210</v>
       </c>
-      <c r="B32" s="139"/>
+      <c r="B32" s="134"/>
       <c r="C32" s="84"/>
-      <c r="D32" s="146"/>
+      <c r="D32" s="131"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="121" t="s">
+      <c r="A33" s="127" t="s">
         <v>610</v>
       </c>
-      <c r="B33" s="121"/>
+      <c r="B33" s="127"/>
       <c r="C33" s="83" t="s">
         <v>615</v>
       </c>
-      <c r="D33" s="146"/>
+      <c r="D33" s="131"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="121"/>
-      <c r="B34" s="121"/>
+      <c r="A34" s="127"/>
+      <c r="B34" s="127"/>
       <c r="C34" s="83" t="s">
         <v>625</v>
       </c>
-      <c r="D34" s="146"/>
+      <c r="D34" s="131"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="136" t="s">
+      <c r="A35" s="129" t="s">
         <v>611</v>
       </c>
-      <c r="B35" s="136"/>
+      <c r="B35" s="129"/>
       <c r="C35" s="84" t="s">
         <v>612</v>
       </c>
-      <c r="D35" s="146"/>
+      <c r="D35" s="131"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="136"/>
-      <c r="B36" s="136"/>
+      <c r="A36" s="129"/>
+      <c r="B36" s="129"/>
       <c r="C36" s="84" t="s">
         <v>613</v>
       </c>
-      <c r="D36" s="146"/>
+      <c r="D36" s="131"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="121" t="s">
+      <c r="A37" s="127" t="s">
         <v>614</v>
       </c>
-      <c r="B37" s="121"/>
+      <c r="B37" s="127"/>
       <c r="C37" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="D37" s="146"/>
+      <c r="D37" s="131"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="121"/>
-      <c r="B38" s="121"/>
+      <c r="A38" s="127"/>
+      <c r="B38" s="127"/>
       <c r="C38" s="83" t="s">
         <v>190</v>
       </c>
-      <c r="D38" s="146"/>
+      <c r="D38" s="131"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="136" t="s">
+      <c r="A39" s="129" t="s">
         <v>621</v>
       </c>
-      <c r="B39" s="136"/>
+      <c r="B39" s="129"/>
       <c r="C39" s="84" t="s">
         <v>616</v>
       </c>
-      <c r="D39" s="146"/>
+      <c r="D39" s="131"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="136"/>
-      <c r="B40" s="136"/>
+      <c r="A40" s="129"/>
+      <c r="B40" s="129"/>
       <c r="C40" s="84" t="s">
         <v>617</v>
       </c>
-      <c r="D40" s="146"/>
+      <c r="D40" s="131"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="121" t="s">
+      <c r="A41" s="127" t="s">
         <v>619</v>
       </c>
-      <c r="B41" s="121"/>
+      <c r="B41" s="127"/>
       <c r="C41" s="83" t="s">
         <v>622</v>
       </c>
-      <c r="D41" s="146"/>
+      <c r="D41" s="131"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="121"/>
-      <c r="B42" s="121"/>
+      <c r="A42" s="127"/>
+      <c r="B42" s="127"/>
       <c r="C42" s="83" t="s">
         <v>623</v>
       </c>
-      <c r="D42" s="146"/>
+      <c r="D42" s="131"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="121"/>
-      <c r="B43" s="121"/>
+      <c r="A43" s="127"/>
+      <c r="B43" s="127"/>
       <c r="C43" s="83" t="s">
         <v>624</v>
       </c>
-      <c r="D43" s="146"/>
+      <c r="D43" s="131"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="121"/>
-      <c r="B44" s="121"/>
+      <c r="A44" s="127"/>
+      <c r="B44" s="127"/>
       <c r="C44" s="83" t="s">
         <v>620</v>
       </c>
-      <c r="D44" s="146"/>
+      <c r="D44" s="131"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="136" t="s">
+      <c r="A45" s="129" t="s">
         <v>626</v>
       </c>
-      <c r="B45" s="136"/>
+      <c r="B45" s="129"/>
       <c r="C45" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="D45" s="146"/>
+      <c r="D45" s="131"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="136"/>
-      <c r="B46" s="136"/>
+      <c r="A46" s="129"/>
+      <c r="B46" s="129"/>
       <c r="C46" s="84" t="s">
         <v>627</v>
       </c>
-      <c r="D46" s="146"/>
+      <c r="D46" s="131"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="136"/>
-      <c r="B47" s="136"/>
+      <c r="A47" s="129"/>
+      <c r="B47" s="129"/>
       <c r="C47" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="D47" s="146"/>
+      <c r="D47" s="131"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="136"/>
-      <c r="B48" s="136"/>
+      <c r="A48" s="129"/>
+      <c r="B48" s="129"/>
       <c r="C48" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="146"/>
+      <c r="D48" s="131"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="136"/>
-      <c r="B49" s="136"/>
+      <c r="A49" s="129"/>
+      <c r="B49" s="129"/>
       <c r="C49" s="84" t="s">
         <v>630</v>
       </c>
-      <c r="D49" s="146"/>
+      <c r="D49" s="131"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="136"/>
-      <c r="B50" s="136"/>
+      <c r="A50" s="129"/>
+      <c r="B50" s="129"/>
       <c r="C50" s="84" t="s">
         <v>628</v>
       </c>
-      <c r="D50" s="146"/>
+      <c r="D50" s="131"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="136"/>
-      <c r="B51" s="136"/>
+      <c r="A51" s="129"/>
+      <c r="B51" s="129"/>
       <c r="C51" s="98" t="s">
         <v>629</v>
       </c>
-      <c r="D51" s="146"/>
+      <c r="D51" s="131"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="121" t="s">
+      <c r="A52" s="127" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="126"/>
+      <c r="B52" s="128"/>
       <c r="C52" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="D52" s="120" t="s">
+      <c r="D52" s="119" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="121"/>
-      <c r="B53" s="126"/>
+      <c r="A53" s="127"/>
+      <c r="B53" s="128"/>
       <c r="C53" s="83" t="s">
         <v>148</v>
       </c>
-      <c r="D53" s="120"/>
+      <c r="D53" s="119"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="121"/>
-      <c r="B54" s="126"/>
+      <c r="A54" s="127"/>
+      <c r="B54" s="128"/>
       <c r="C54" s="83" t="s">
         <v>149</v>
       </c>
-      <c r="D54" s="120"/>
+      <c r="D54" s="119"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="121"/>
-      <c r="B55" s="126"/>
+      <c r="A55" s="127"/>
+      <c r="B55" s="128"/>
       <c r="C55" s="84" t="s">
         <v>636</v>
       </c>
-      <c r="D55" s="119" t="s">
+      <c r="D55" s="120" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="121"/>
-      <c r="B56" s="126"/>
+      <c r="A56" s="127"/>
+      <c r="B56" s="128"/>
       <c r="C56" s="84" t="s">
         <v>143</v>
       </c>
-      <c r="D56" s="119"/>
+      <c r="D56" s="120"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="121"/>
-      <c r="B57" s="126"/>
+      <c r="A57" s="127"/>
+      <c r="B57" s="128"/>
       <c r="C57" s="84" t="s">
         <v>141</v>
       </c>
-      <c r="D57" s="119"/>
+      <c r="D57" s="120"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="121"/>
-      <c r="B58" s="126"/>
+      <c r="A58" s="127"/>
+      <c r="B58" s="128"/>
       <c r="C58" s="84" t="s">
         <v>144</v>
       </c>
-      <c r="D58" s="119"/>
+      <c r="D58" s="120"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="121"/>
-      <c r="B59" s="126"/>
+      <c r="A59" s="127"/>
+      <c r="B59" s="128"/>
       <c r="C59" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="D59" s="119"/>
+      <c r="D59" s="120"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="121"/>
-      <c r="B60" s="126"/>
+      <c r="A60" s="127"/>
+      <c r="B60" s="128"/>
       <c r="C60" s="84" t="s">
         <v>146</v>
       </c>
-      <c r="D60" s="119"/>
+      <c r="D60" s="120"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="121"/>
-      <c r="B61" s="126"/>
+      <c r="A61" s="127"/>
+      <c r="B61" s="128"/>
       <c r="C61" s="83" t="s">
         <v>335</v>
       </c>
@@ -7510,76 +7525,76 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="121"/>
-      <c r="B62" s="126"/>
+      <c r="A62" s="127"/>
+      <c r="B62" s="128"/>
       <c r="C62" s="84" t="s">
         <v>637</v>
       </c>
-      <c r="D62" s="127" t="s">
+      <c r="D62" s="121" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="121"/>
-      <c r="B63" s="126"/>
+      <c r="A63" s="127"/>
+      <c r="B63" s="128"/>
       <c r="C63" s="84" t="s">
         <v>638</v>
       </c>
-      <c r="D63" s="128"/>
+      <c r="D63" s="140"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="121"/>
-      <c r="B64" s="126"/>
+      <c r="A64" s="127"/>
+      <c r="B64" s="128"/>
       <c r="C64" s="83" t="s">
         <v>589</v>
       </c>
-      <c r="D64" s="132" t="s">
+      <c r="D64" s="137" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A65" s="121"/>
-      <c r="B65" s="126"/>
+      <c r="A65" s="127"/>
+      <c r="B65" s="128"/>
       <c r="C65" s="83" t="s">
         <v>590</v>
       </c>
-      <c r="D65" s="135"/>
+      <c r="D65" s="138"/>
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A66" s="121"/>
-      <c r="B66" s="126"/>
+      <c r="A66" s="127"/>
+      <c r="B66" s="128"/>
       <c r="C66" s="83" t="s">
         <v>591</v>
       </c>
-      <c r="D66" s="135"/>
+      <c r="D66" s="138"/>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A67" s="121"/>
-      <c r="B67" s="126"/>
+      <c r="A67" s="127"/>
+      <c r="B67" s="128"/>
       <c r="C67" s="83" t="s">
         <v>592</v>
       </c>
-      <c r="D67" s="135"/>
+      <c r="D67" s="138"/>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A68" s="121"/>
-      <c r="B68" s="126"/>
+      <c r="A68" s="127"/>
+      <c r="B68" s="128"/>
       <c r="C68" s="83" t="s">
         <v>639</v>
       </c>
-      <c r="D68" s="135"/>
+      <c r="D68" s="138"/>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A69" s="121"/>
-      <c r="B69" s="126"/>
+      <c r="A69" s="127"/>
+      <c r="B69" s="128"/>
       <c r="C69" s="83" t="s">
         <v>594</v>
       </c>
-      <c r="D69" s="131"/>
+      <c r="D69" s="139"/>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A70" s="121"/>
-      <c r="B70" s="126"/>
+      <c r="A70" s="127"/>
+      <c r="B70" s="128"/>
       <c r="C70" s="84" t="s">
         <v>597</v>
       </c>
@@ -7588,105 +7603,105 @@
       </c>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A71" s="137" t="s">
+      <c r="A71" s="132" t="s">
         <v>634</v>
       </c>
-      <c r="B71" s="137"/>
+      <c r="B71" s="132"/>
       <c r="C71" s="101" t="s">
         <v>178</v>
       </c>
-      <c r="D71" s="133" t="s">
+      <c r="D71" s="135" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A72" s="137"/>
-      <c r="B72" s="137"/>
+      <c r="A72" s="132"/>
+      <c r="B72" s="132"/>
       <c r="C72" s="102" t="s">
         <v>179</v>
       </c>
-      <c r="D72" s="134"/>
+      <c r="D72" s="136"/>
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A73" s="120" t="s">
+      <c r="A73" s="119" t="s">
         <v>633</v>
       </c>
-      <c r="B73" s="120"/>
+      <c r="B73" s="119"/>
       <c r="C73" s="83" t="s">
         <v>632</v>
       </c>
-      <c r="D73" s="120" t="s">
+      <c r="D73" s="119" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A74" s="120"/>
-      <c r="B74" s="120"/>
+      <c r="A74" s="119"/>
+      <c r="B74" s="119"/>
       <c r="C74" s="83" t="s">
         <v>221</v>
       </c>
-      <c r="D74" s="120"/>
+      <c r="D74" s="119"/>
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A75" s="119" t="s">
+      <c r="A75" s="120" t="s">
         <v>635</v>
       </c>
-      <c r="B75" s="119"/>
+      <c r="B75" s="120"/>
       <c r="C75" s="84" t="s">
         <v>616</v>
       </c>
-      <c r="D75" s="119" t="s">
+      <c r="D75" s="120" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A76" s="119"/>
-      <c r="B76" s="119"/>
+      <c r="A76" s="120"/>
+      <c r="B76" s="120"/>
       <c r="C76" s="84" t="s">
         <v>617</v>
       </c>
-      <c r="D76" s="119"/>
+      <c r="D76" s="120"/>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A77" s="120" t="s">
+      <c r="A77" s="119" t="s">
         <v>640</v>
       </c>
-      <c r="B77" s="120"/>
+      <c r="B77" s="119"/>
       <c r="C77" s="83" t="s">
         <v>641</v>
       </c>
-      <c r="D77" s="120" t="s">
+      <c r="D77" s="119" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A78" s="120"/>
-      <c r="B78" s="120"/>
+      <c r="A78" s="119"/>
+      <c r="B78" s="119"/>
       <c r="C78" s="83" t="s">
         <v>642</v>
       </c>
-      <c r="D78" s="120"/>
+      <c r="D78" s="119"/>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A79" s="120"/>
-      <c r="B79" s="120"/>
+      <c r="A79" s="119"/>
+      <c r="B79" s="119"/>
       <c r="C79" s="83" t="s">
         <v>643</v>
       </c>
-      <c r="D79" s="120"/>
+      <c r="D79" s="119"/>
       <c r="W79"/>
       <c r="AD79" s="38"/>
       <c r="AE79"/>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A80" s="119" t="s">
+      <c r="A80" s="120" t="s">
         <v>646</v>
       </c>
-      <c r="B80" s="119"/>
+      <c r="B80" s="120"/>
       <c r="C80" s="104" t="s">
         <v>293</v>
       </c>
-      <c r="D80" s="127" t="s">
+      <c r="D80" s="121" t="s">
         <v>629</v>
       </c>
       <c r="W80"/>
@@ -7694,283 +7709,283 @@
       <c r="AE80"/>
     </row>
     <row r="81" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A81" s="119"/>
-      <c r="B81" s="119"/>
+      <c r="A81" s="120"/>
+      <c r="B81" s="120"/>
       <c r="C81" s="84" t="s">
         <v>294</v>
       </c>
-      <c r="D81" s="128"/>
+      <c r="D81" s="140"/>
     </row>
     <row r="82" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A82" s="131" t="s">
+      <c r="A82" s="139" t="s">
         <v>647</v>
       </c>
-      <c r="B82" s="131"/>
+      <c r="B82" s="139"/>
       <c r="C82" s="113" t="s">
         <v>194</v>
       </c>
-      <c r="D82" s="129"/>
+      <c r="D82" s="141"/>
       <c r="W82"/>
       <c r="AD82" s="38"/>
       <c r="AE82"/>
     </row>
     <row r="83" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A83" s="132"/>
-      <c r="B83" s="132"/>
+      <c r="A83" s="137"/>
+      <c r="B83" s="137"/>
       <c r="C83" s="112" t="s">
         <v>195</v>
       </c>
-      <c r="D83" s="130"/>
+      <c r="D83" s="142"/>
     </row>
     <row r="84" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A84" s="119" t="s">
+      <c r="A84" s="120" t="s">
         <v>648</v>
       </c>
-      <c r="B84" s="119"/>
+      <c r="B84" s="120"/>
       <c r="C84" s="84" t="s">
         <v>657</v>
       </c>
-      <c r="D84" s="119" t="s">
+      <c r="D84" s="120" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="85" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A85" s="119"/>
-      <c r="B85" s="119"/>
+      <c r="A85" s="120"/>
+      <c r="B85" s="120"/>
       <c r="C85" s="84" t="s">
         <v>656</v>
       </c>
-      <c r="D85" s="119"/>
+      <c r="D85" s="120"/>
     </row>
     <row r="86" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A86" s="119" t="s">
+      <c r="A86" s="120" t="s">
         <v>650</v>
       </c>
-      <c r="B86" s="119"/>
+      <c r="B86" s="120"/>
       <c r="C86" s="84" t="s">
         <v>651</v>
       </c>
-      <c r="D86" s="119"/>
+      <c r="D86" s="120"/>
     </row>
     <row r="87" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A87" s="119"/>
-      <c r="B87" s="119"/>
+      <c r="A87" s="120"/>
+      <c r="B87" s="120"/>
       <c r="C87" s="84" t="s">
         <v>652</v>
       </c>
-      <c r="D87" s="119"/>
+      <c r="D87" s="120"/>
     </row>
     <row r="88" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A88" s="119" t="s">
+      <c r="A88" s="120" t="s">
         <v>653</v>
       </c>
-      <c r="B88" s="119"/>
+      <c r="B88" s="120"/>
       <c r="C88" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="D88" s="119"/>
+      <c r="D88" s="120"/>
     </row>
     <row r="89" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A89" s="119"/>
-      <c r="B89" s="119"/>
+      <c r="A89" s="120"/>
+      <c r="B89" s="120"/>
       <c r="C89" s="84" t="s">
         <v>655</v>
       </c>
-      <c r="D89" s="119"/>
+      <c r="D89" s="120"/>
     </row>
     <row r="90" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A90" s="120" t="s">
+      <c r="A90" s="119" t="s">
         <v>659</v>
       </c>
-      <c r="B90" s="120"/>
+      <c r="B90" s="119"/>
       <c r="C90" s="83" t="s">
         <v>645</v>
       </c>
     </row>
     <row r="91" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A91" s="120"/>
-      <c r="B91" s="120"/>
+      <c r="A91" s="119"/>
+      <c r="B91" s="119"/>
       <c r="C91" s="83" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="92" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A92" s="119" t="s">
+      <c r="A92" s="120" t="s">
         <v>660</v>
       </c>
-      <c r="B92" s="119"/>
+      <c r="B92" s="120"/>
       <c r="C92" s="84" t="s">
         <v>662</v>
       </c>
       <c r="AQ92" s="9"/>
     </row>
     <row r="93" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A93" s="119"/>
-      <c r="B93" s="119"/>
+      <c r="A93" s="120"/>
+      <c r="B93" s="120"/>
       <c r="C93" s="84" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="94" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A94" s="127"/>
-      <c r="B94" s="127"/>
+      <c r="A94" s="121"/>
+      <c r="B94" s="121"/>
       <c r="C94" s="98" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="95" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A95" s="120" t="s">
+      <c r="A95" s="119" t="s">
         <v>664</v>
       </c>
-      <c r="B95" s="120"/>
+      <c r="B95" s="119"/>
       <c r="C95" s="83" t="s">
         <v>665</v>
       </c>
-      <c r="D95" s="120" t="s">
+      <c r="D95" s="119" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="96" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A96" s="120"/>
-      <c r="B96" s="120"/>
+      <c r="A96" s="119"/>
+      <c r="B96" s="119"/>
       <c r="C96" s="83" t="s">
         <v>666</v>
       </c>
-      <c r="D96" s="120"/>
+      <c r="D96" s="119"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="119" t="s">
+      <c r="A97" s="120" t="s">
         <v>667</v>
       </c>
-      <c r="B97" s="119"/>
+      <c r="B97" s="120"/>
       <c r="C97" s="84" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="119"/>
-      <c r="B98" s="119"/>
+      <c r="A98" s="120"/>
+      <c r="B98" s="120"/>
       <c r="C98" s="84" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="120" t="s">
+      <c r="A99" s="119" t="s">
         <v>668</v>
       </c>
-      <c r="B99" s="120"/>
+      <c r="B99" s="119"/>
       <c r="C99" s="83" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="120"/>
-      <c r="B100" s="120"/>
+      <c r="A100" s="119"/>
+      <c r="B100" s="119"/>
       <c r="C100" s="83" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="119" t="s">
+      <c r="A101" s="120" t="s">
         <v>669</v>
       </c>
-      <c r="B101" s="119"/>
+      <c r="B101" s="120"/>
       <c r="C101" s="84" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="119"/>
-      <c r="B102" s="119"/>
+      <c r="A102" s="120"/>
+      <c r="B102" s="120"/>
       <c r="C102" s="84" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="121" t="s">
+      <c r="A103" s="127" t="s">
         <v>671</v>
       </c>
-      <c r="B103" s="126"/>
+      <c r="B103" s="128"/>
       <c r="C103" s="115" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="121"/>
-      <c r="B104" s="126"/>
+      <c r="A104" s="127"/>
+      <c r="B104" s="128"/>
       <c r="C104" s="112" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="119" t="s">
+      <c r="A105" s="120" t="s">
         <v>673</v>
       </c>
-      <c r="B105" s="119"/>
+      <c r="B105" s="120"/>
       <c r="C105" s="84" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="119"/>
-      <c r="B106" s="119"/>
+      <c r="A106" s="120"/>
+      <c r="B106" s="120"/>
       <c r="C106" s="84" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="120" t="s">
+      <c r="A107" s="119" t="s">
         <v>672</v>
       </c>
-      <c r="B107" s="120"/>
+      <c r="B107" s="119"/>
       <c r="C107" s="83" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="120"/>
-      <c r="B108" s="120"/>
+      <c r="A108" s="119"/>
+      <c r="B108" s="119"/>
       <c r="C108" s="83" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="119" t="s">
+      <c r="A109" s="120" t="s">
         <v>674</v>
       </c>
-      <c r="B109" s="119"/>
+      <c r="B109" s="120"/>
       <c r="C109" s="84" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="119"/>
-      <c r="B110" s="119"/>
+      <c r="A110" s="120"/>
+      <c r="B110" s="120"/>
       <c r="C110" s="84" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="120" t="s">
+      <c r="A111" s="119" t="s">
         <v>675</v>
       </c>
-      <c r="B111" s="120"/>
+      <c r="B111" s="119"/>
       <c r="C111" s="83" t="s">
         <v>677</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="120"/>
-      <c r="B112" s="120"/>
+      <c r="A112" s="119"/>
+      <c r="B112" s="119"/>
       <c r="C112" s="83" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="119" t="s">
+      <c r="A113" s="120" t="s">
         <v>678</v>
       </c>
-      <c r="B113" s="119"/>
+      <c r="B113" s="120"/>
       <c r="C113" s="84" t="s">
         <v>632</v>
       </c>
@@ -7979,107 +7994,107 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="119"/>
-      <c r="B114" s="119"/>
+      <c r="A114" s="120"/>
+      <c r="B114" s="120"/>
       <c r="C114" s="84" t="s">
         <v>221</v>
       </c>
       <c r="D114" s="84"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="120" t="s">
+      <c r="A115" s="119" t="s">
         <v>680</v>
       </c>
-      <c r="B115" s="120"/>
+      <c r="B115" s="119"/>
       <c r="C115" s="83" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="120"/>
-      <c r="B116" s="120"/>
+      <c r="A116" s="119"/>
+      <c r="B116" s="119"/>
       <c r="C116" s="83" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="120"/>
-      <c r="B117" s="120"/>
+      <c r="A117" s="119"/>
+      <c r="B117" s="119"/>
       <c r="C117" s="83" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="122" t="s">
+      <c r="A118" s="143" t="s">
         <v>681</v>
       </c>
-      <c r="B118" s="123"/>
+      <c r="B118" s="144"/>
       <c r="C118" s="84" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="124"/>
-      <c r="B119" s="125"/>
+      <c r="A119" s="145"/>
+      <c r="B119" s="146"/>
       <c r="C119" s="84" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="120" t="s">
+      <c r="A120" s="119" t="s">
         <v>682</v>
       </c>
-      <c r="B120" s="120"/>
+      <c r="B120" s="119"/>
       <c r="C120" s="83" t="s">
         <v>632</v>
       </c>
-      <c r="D120" s="121" t="s">
+      <c r="D120" s="127" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="120"/>
-      <c r="B121" s="120"/>
+      <c r="A121" s="119"/>
+      <c r="B121" s="119"/>
       <c r="C121" s="83" t="s">
         <v>221</v>
       </c>
-      <c r="D121" s="121"/>
+      <c r="D121" s="127"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="119" t="s">
+      <c r="A122" s="120" t="s">
         <v>683</v>
       </c>
-      <c r="B122" s="119"/>
+      <c r="B122" s="120"/>
       <c r="C122" s="84" t="s">
         <v>632</v>
       </c>
-      <c r="D122" s="121"/>
+      <c r="D122" s="127"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="119"/>
-      <c r="B123" s="119"/>
+      <c r="A123" s="120"/>
+      <c r="B123" s="120"/>
       <c r="C123" s="84" t="s">
         <v>221</v>
       </c>
-      <c r="D123" s="121"/>
+      <c r="D123" s="127"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="120" t="s">
+      <c r="A124" s="119" t="s">
         <v>684</v>
       </c>
-      <c r="B124" s="120"/>
+      <c r="B124" s="119"/>
       <c r="C124" s="83" t="s">
         <v>632</v>
       </c>
-      <c r="D124" s="121"/>
+      <c r="D124" s="127"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="120"/>
-      <c r="B125" s="120"/>
+      <c r="A125" s="119"/>
+      <c r="B125" s="119"/>
       <c r="C125" s="83" t="s">
         <v>221</v>
       </c>
-      <c r="D125" s="121"/>
+      <c r="D125" s="127"/>
     </row>
     <row r="155" spans="28:31" x14ac:dyDescent="0.3">
       <c r="AB155" s="29"/>
@@ -8136,12 +8151,39 @@
   </sheetData>
   <autoFilter ref="A1:FQ153" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}"/>
   <mergeCells count="55">
-    <mergeCell ref="A99:B100"/>
-    <mergeCell ref="A90:B91"/>
-    <mergeCell ref="A92:B94"/>
-    <mergeCell ref="A95:B96"/>
-    <mergeCell ref="D95:D96"/>
-    <mergeCell ref="A97:B98"/>
+    <mergeCell ref="A122:B123"/>
+    <mergeCell ref="A124:B125"/>
+    <mergeCell ref="D120:D125"/>
+    <mergeCell ref="A111:B112"/>
+    <mergeCell ref="A113:B114"/>
+    <mergeCell ref="A115:B117"/>
+    <mergeCell ref="A118:B119"/>
+    <mergeCell ref="A120:B121"/>
+    <mergeCell ref="A101:B102"/>
+    <mergeCell ref="A103:B104"/>
+    <mergeCell ref="A105:B106"/>
+    <mergeCell ref="A107:B108"/>
+    <mergeCell ref="A109:B110"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="D84:D89"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="A80:B81"/>
+    <mergeCell ref="A82:B83"/>
+    <mergeCell ref="A84:B85"/>
+    <mergeCell ref="A86:B87"/>
+    <mergeCell ref="A88:B89"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D64:D69"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A52:B70"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="D55:D60"/>
+    <mergeCell ref="A35:B36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="A71:B72"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A73:B74"/>
     <mergeCell ref="A77:B79"/>
     <mergeCell ref="D77:D79"/>
     <mergeCell ref="A21:D21"/>
@@ -8158,39 +8200,12 @@
     <mergeCell ref="A28:B29"/>
     <mergeCell ref="A30:B31"/>
     <mergeCell ref="A33:B34"/>
-    <mergeCell ref="A35:B36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="A71:B72"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A73:B74"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="D64:D69"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A52:B70"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="D55:D60"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="D84:D89"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="A80:B81"/>
-    <mergeCell ref="A82:B83"/>
-    <mergeCell ref="A84:B85"/>
-    <mergeCell ref="A86:B87"/>
-    <mergeCell ref="A88:B89"/>
-    <mergeCell ref="A101:B102"/>
-    <mergeCell ref="A103:B104"/>
-    <mergeCell ref="A105:B106"/>
-    <mergeCell ref="A107:B108"/>
-    <mergeCell ref="A109:B110"/>
-    <mergeCell ref="A122:B123"/>
-    <mergeCell ref="A124:B125"/>
-    <mergeCell ref="D120:D125"/>
-    <mergeCell ref="A111:B112"/>
-    <mergeCell ref="A113:B114"/>
-    <mergeCell ref="A115:B117"/>
-    <mergeCell ref="A118:B119"/>
-    <mergeCell ref="A120:B121"/>
+    <mergeCell ref="A99:B100"/>
+    <mergeCell ref="A90:B91"/>
+    <mergeCell ref="A92:B94"/>
+    <mergeCell ref="A95:B96"/>
+    <mergeCell ref="D95:D96"/>
+    <mergeCell ref="A97:B98"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -12062,6 +12077,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="1a0cd919-d361-40f9-9afc-7bc6ff95d333" xsi:nil="true"/>
@@ -12070,15 +12094,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12277,6 +12292,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C1A5563-A825-4419-97ED-5452D9012A3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -12289,14 +12312,6 @@
     <ds:schemaRef ds:uri="67252fe7-6b63-4403-af0d-37df51d7c3a2"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Changement de version 9.7.4 et adaptation
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbenjemi\Katalon Studio\ANEF_Eloignement_V1_Nawres\ANEF-Eloignement\ANEF_Eloignement_V1_Nawres\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EAF59C-7DF0-4806-B29E-825F3313E47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C35AE5-2CFC-4A6B-8D89-0DD6135FAD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="694">
   <si>
     <t>URL_ANEFdevfenv5</t>
   </si>
@@ -2059,9 +2059,6 @@
     <t>AjouterJLD</t>
   </si>
   <si>
-    <t>NbreJLD</t>
-  </si>
-  <si>
     <t>AjouterVisiteDomiciliare</t>
   </si>
   <si>
@@ -2123,6 +2120,15 @@
   </si>
   <si>
     <t>L 731-3 6°</t>
+  </si>
+  <si>
+    <t>NombreJLD</t>
+  </si>
+  <si>
+    <t>AjouterRecoursContentieux</t>
+  </si>
+  <si>
+    <t>Mesure != Expulsion</t>
   </si>
 </sst>
 </file>
@@ -2604,7 +2610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3027,6 +3033,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3342,10 +3351,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}">
   <dimension ref="A1:FS173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AH1" sqref="AH1"/>
-      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3503,54 +3512,56 @@
         <v>668</v>
       </c>
       <c r="AB1" s="115" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AC1" s="86" t="s">
         <v>669</v>
       </c>
       <c r="AD1" s="86" t="s">
+        <v>691</v>
+      </c>
+      <c r="AE1" s="86" t="s">
         <v>670</v>
       </c>
-      <c r="AE1" s="86" t="s">
+      <c r="AF1" s="86" t="s">
+        <v>682</v>
+      </c>
+      <c r="AG1" s="86" t="s">
         <v>671</v>
       </c>
-      <c r="AF1" s="86" t="s">
+      <c r="AH1" s="86" t="s">
+        <v>672</v>
+      </c>
+      <c r="AI1" s="86" t="s">
         <v>683</v>
       </c>
-      <c r="AG1" s="86" t="s">
-        <v>672</v>
-      </c>
-      <c r="AH1" s="86" t="s">
+      <c r="AJ1" s="86" t="s">
         <v>673</v>
       </c>
-      <c r="AI1" s="86" t="s">
-        <v>684</v>
-      </c>
-      <c r="AJ1" s="86" t="s">
+      <c r="AK1" s="86" t="s">
         <v>674</v>
       </c>
-      <c r="AK1" s="86" t="s">
+      <c r="AL1" s="86" t="s">
         <v>675</v>
       </c>
-      <c r="AL1" s="86" t="s">
-        <v>676</v>
-      </c>
       <c r="AM1" s="86" t="s">
+        <v>677</v>
+      </c>
+      <c r="AN1" s="23" t="s">
         <v>678</v>
       </c>
-      <c r="AN1" s="23" t="s">
+      <c r="AO1" s="23" t="s">
         <v>679</v>
       </c>
-      <c r="AO1" s="23" t="s">
+      <c r="AP1" s="23" t="s">
         <v>680</v>
       </c>
-      <c r="AP1" s="23" t="s">
+      <c r="AQ1" s="23" t="s">
         <v>681</v>
       </c>
-      <c r="AQ1" s="23" t="s">
-        <v>682</v>
-      </c>
-      <c r="AR1" s="23"/>
+      <c r="AR1" s="23" t="s">
+        <v>692</v>
+      </c>
       <c r="AS1" s="13"/>
       <c r="AT1" s="13"/>
       <c r="AU1" s="13"/>
@@ -3695,10 +3706,10 @@
         <v>658</v>
       </c>
       <c r="E2" s="106" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F2" s="106">
-        <v>7503182107</v>
+        <v>7503182266</v>
       </c>
       <c r="G2" s="106" t="s">
         <v>615</v>
@@ -3758,7 +3769,7 @@
         <v>632</v>
       </c>
       <c r="AD2" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AE2" s="115" t="s">
         <v>221</v>
@@ -3777,7 +3788,7 @@
         <v>632</v>
       </c>
       <c r="AK2" s="104" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="AL2" s="104" t="s">
         <v>632</v>
@@ -4233,13 +4244,13 @@
         <v>221</v>
       </c>
       <c r="AI4" s="104" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="AJ4" s="104" t="s">
         <v>221</v>
       </c>
       <c r="AK4" s="104" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="AL4" s="104" t="s">
         <v>221</v>
@@ -4460,17 +4471,17 @@
       <c r="AG5" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="AH5" s="11" t="s">
+      <c r="AH5" s="104" t="s">
         <v>632</v>
       </c>
       <c r="AI5" s="104" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="AJ5" s="104" t="s">
         <v>632</v>
       </c>
       <c r="AK5" s="104" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="AL5" s="104" t="s">
         <v>221</v>
@@ -4614,19 +4625,19 @@
         <v>74</v>
       </c>
       <c r="B6" s="104" t="s">
-        <v>76</v>
+        <v>599</v>
       </c>
       <c r="C6" s="105" t="s">
-        <v>631</v>
+        <v>644</v>
       </c>
       <c r="D6" s="105" t="s">
-        <v>187</v>
+        <v>658</v>
       </c>
       <c r="E6" s="106" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F6" s="106">
-        <v>7703056080</v>
+        <v>7503182087</v>
       </c>
       <c r="G6" s="106" t="s">
         <v>625</v>
@@ -4668,36 +4679,54 @@
         <v>645</v>
       </c>
       <c r="X6" s="113" t="s">
-        <v>662</v>
-      </c>
-      <c r="Y6" s="104" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
+        <v>663</v>
+      </c>
+      <c r="Y6" s="104"/>
+      <c r="Z6" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB6" s="73"/>
       <c r="AC6" s="28"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="28"/>
       <c r="AF6" s="28"/>
       <c r="AG6" s="2"/>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="11"/>
-      <c r="AJ6" s="11"/>
-      <c r="AK6" s="11"/>
-      <c r="AL6" s="11"/>
-      <c r="AM6" s="11"/>
-      <c r="AN6" s="11"/>
+      <c r="AH6" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI6" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ6" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AK6" s="104" t="s">
+        <v>686</v>
+      </c>
+      <c r="AL6" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM6" s="104" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN6" s="104" t="s">
+        <v>632</v>
+      </c>
       <c r="AO6" s="104" t="s">
         <v>221</v>
       </c>
       <c r="AP6" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="AQ6" s="116" t="s">
+        <v>221</v>
+      </c>
+      <c r="AR6" s="147" t="s">
         <v>632</v>
       </c>
-      <c r="AQ6" s="116" t="s">
-        <v>632</v>
-      </c>
-      <c r="AR6" s="12"/>
       <c r="AS6" s="11"/>
       <c r="AT6" s="28"/>
       <c r="AU6" s="28"/>
@@ -4839,7 +4868,7 @@
         <v>609</v>
       </c>
       <c r="F7" s="106">
-        <v>7703056080</v>
+        <v>7503182087</v>
       </c>
       <c r="G7" s="106" t="s">
         <v>625</v>
@@ -4877,11 +4906,19 @@
       <c r="T7" s="84"/>
       <c r="U7" s="84"/>
       <c r="V7" s="84"/>
-      <c r="W7" s="84"/>
-      <c r="X7" s="28"/>
+      <c r="W7" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X7" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y7" s="11"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
+      <c r="Z7" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB7" s="73"/>
       <c r="AC7" s="28"/>
       <c r="AD7" s="2"/>
@@ -5074,11 +5111,19 @@
       <c r="T8" s="84"/>
       <c r="U8" s="84"/>
       <c r="V8" s="84"/>
-      <c r="W8" s="84"/>
-      <c r="X8" s="28"/>
+      <c r="W8" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X8" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y8" s="11"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
+      <c r="Z8" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB8" s="73"/>
       <c r="AC8" s="28"/>
       <c r="AD8" s="2"/>
@@ -5273,11 +5318,19 @@
       <c r="T9" s="84"/>
       <c r="U9" s="84"/>
       <c r="V9" s="84"/>
-      <c r="W9" s="84"/>
-      <c r="X9" s="28"/>
+      <c r="W9" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X9" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y9" s="11"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
+      <c r="Z9" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB9" s="73"/>
       <c r="AC9" s="28"/>
       <c r="AD9" s="2"/>
@@ -5470,14 +5523,26 @@
       <c r="T10" s="84"/>
       <c r="U10" s="84"/>
       <c r="V10" s="84"/>
-      <c r="W10" s="84"/>
-      <c r="X10" s="28"/>
+      <c r="W10" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X10" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y10" s="11"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
+      <c r="Z10" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB10" s="73"/>
-      <c r="AC10" s="28"/>
-      <c r="AD10" s="2"/>
+      <c r="AC10" s="28" t="s">
+        <v>632</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>2</v>
+      </c>
       <c r="AE10" s="28"/>
       <c r="AF10" s="28"/>
       <c r="AG10" s="2"/>
@@ -5667,11 +5732,19 @@
       <c r="T11" s="84"/>
       <c r="U11" s="84"/>
       <c r="V11" s="84"/>
-      <c r="W11" s="84"/>
-      <c r="X11" s="28"/>
+      <c r="W11" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X11" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y11" s="11"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
+      <c r="Z11" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB11" s="73"/>
       <c r="AC11" s="28"/>
       <c r="AD11" s="2"/>
@@ -5862,11 +5935,19 @@
       <c r="T12" s="84"/>
       <c r="U12" s="84"/>
       <c r="V12" s="84"/>
-      <c r="W12" s="84"/>
-      <c r="X12" s="28"/>
+      <c r="W12" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X12" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y12" s="11"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
+      <c r="Z12" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB12" s="73"/>
       <c r="AC12" s="28"/>
       <c r="AD12" s="2"/>
@@ -6057,11 +6138,19 @@
       <c r="T13" s="84"/>
       <c r="U13" s="84"/>
       <c r="V13" s="84"/>
-      <c r="W13" s="84"/>
-      <c r="X13" s="28"/>
+      <c r="W13" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X13" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y13" s="11"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
+      <c r="Z13" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB13" s="73"/>
       <c r="AC13" s="28"/>
       <c r="AD13" s="2"/>
@@ -6258,14 +6347,26 @@
       <c r="V14" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="W14" s="84"/>
-      <c r="X14" s="28"/>
+      <c r="W14" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X14" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y14" s="11"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
+      <c r="Z14" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB14" s="73"/>
-      <c r="AC14" s="28"/>
-      <c r="AD14" s="2"/>
+      <c r="AC14" s="28" t="s">
+        <v>632</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>7</v>
+      </c>
       <c r="AE14" s="28"/>
       <c r="AF14" s="28"/>
       <c r="AG14" s="2"/>
@@ -6459,11 +6560,19 @@
       <c r="V15" s="84" t="s">
         <v>655</v>
       </c>
-      <c r="W15" s="84"/>
-      <c r="X15" s="28"/>
+      <c r="W15" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X15" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y15" s="11"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
+      <c r="Z15" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB15" s="73"/>
       <c r="AC15" s="28"/>
       <c r="AD15" s="2"/>
@@ -6658,11 +6767,19 @@
       <c r="V16" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="W16" s="84"/>
-      <c r="X16" s="28"/>
+      <c r="W16" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X16" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y16" s="11"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
+      <c r="Z16" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB16" s="73"/>
       <c r="AC16" s="28"/>
       <c r="AD16" s="2"/>
@@ -6855,11 +6972,19 @@
       <c r="V17" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="W17" s="84"/>
-      <c r="X17" s="28"/>
+      <c r="W17" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X17" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y17" s="11"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
+      <c r="Z17" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB17" s="73"/>
       <c r="AC17" s="28"/>
       <c r="AD17" s="2"/>
@@ -7054,11 +7179,19 @@
       <c r="V18" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="W18" s="84"/>
-      <c r="X18" s="28"/>
+      <c r="W18" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X18" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y18" s="11"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
+      <c r="Z18" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB18" s="73"/>
       <c r="AC18" s="28"/>
       <c r="AD18" s="2"/>
@@ -7201,14 +7334,10 @@
       <c r="FP18" s="78"/>
     </row>
     <row r="19" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="AG19"/>
       <c r="AH19" s="37"/>
-      <c r="AI19" s="37"/>
     </row>
     <row r="20" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="AG20"/>
       <c r="AH20" s="37"/>
-      <c r="AI20" s="37"/>
     </row>
     <row r="21" spans="1:172" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="120" t="s">
@@ -7971,7 +8100,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="125" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B103" s="126"/>
       <c r="C103" s="114" t="s">
@@ -7987,7 +8116,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="118" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B105" s="118"/>
       <c r="C105" s="83" t="s">
@@ -8003,7 +8132,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="117" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B107" s="117"/>
       <c r="C107" s="82" t="s">
@@ -8019,7 +8148,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="118" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B109" s="118"/>
       <c r="C109" s="83" t="s">
@@ -8035,30 +8164,30 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="117" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B111" s="117"/>
       <c r="C111" s="82" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="117"/>
       <c r="B112" s="117"/>
       <c r="C112" s="82" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="118" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B113" s="118"/>
       <c r="C113" s="83" t="s">
         <v>632</v>
       </c>
       <c r="D113" s="83" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -8071,7 +8200,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="117" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B115" s="117"/>
       <c r="C115" s="82" t="s">
@@ -8094,7 +8223,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="141" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B118" s="142"/>
       <c r="C118" s="83" t="s">
@@ -8110,7 +8239,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="117" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B120" s="117"/>
       <c r="C120" s="82" t="s">
@@ -8130,7 +8259,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="118" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B122" s="118"/>
       <c r="C122" s="83" t="s">
@@ -8148,7 +8277,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="117" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B124" s="117"/>
       <c r="C124" s="82" t="s">
@@ -8166,7 +8295,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="145" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B126" s="142"/>
       <c r="C126" s="83" t="s">
@@ -8186,63 +8315,83 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="117" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B128" s="117"/>
       <c r="C128" s="82" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="117"/>
       <c r="B129" s="117"/>
       <c r="C129" s="82" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="117"/>
       <c r="B130" s="117"/>
       <c r="C130" s="82" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="118" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B131" s="118"/>
       <c r="C131" s="83" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="118"/>
       <c r="B132" s="118"/>
       <c r="C132" s="83" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="118"/>
       <c r="B133" s="118"/>
       <c r="C133" s="83" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="118"/>
       <c r="B134" s="118"/>
       <c r="C134" s="83" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" s="118"/>
-      <c r="B135" s="118"/>
-      <c r="C135" s="83" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="119"/>
+      <c r="B135" s="119"/>
+      <c r="C135" s="97" t="s">
         <v>666</v>
       </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="117" t="s">
+        <v>692</v>
+      </c>
+      <c r="B136" s="117"/>
+      <c r="C136" s="82" t="s">
+        <v>632</v>
+      </c>
+      <c r="D136" s="117" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="117"/>
+      <c r="B137" s="117"/>
+      <c r="C137" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="D137" s="117"/>
     </row>
     <row r="155" spans="29:33" x14ac:dyDescent="0.3">
       <c r="AC155" s="28"/>
@@ -8299,11 +8448,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:FS153" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}"/>
-  <mergeCells count="59">
+  <mergeCells count="61">
     <mergeCell ref="A126:B127"/>
     <mergeCell ref="D126:D127"/>
     <mergeCell ref="A128:B130"/>
     <mergeCell ref="A131:B135"/>
+    <mergeCell ref="A136:B137"/>
+    <mergeCell ref="D136:D137"/>
     <mergeCell ref="A122:B123"/>
     <mergeCell ref="A124:B125"/>
     <mergeCell ref="D120:D125"/>
@@ -8377,9 +8528,10 @@
     <hyperlink ref="C13" r:id="rId13" xr:uid="{F90A0876-BE67-43B0-9F92-5AA5FA687F8D}"/>
     <hyperlink ref="C3" r:id="rId14" xr:uid="{A67AD39C-DE35-456E-A0B9-16F23679CB74}"/>
     <hyperlink ref="C4" r:id="rId15" xr:uid="{644DC2C3-754F-4CB6-9E7B-D46B3B117263}"/>
+    <hyperlink ref="C6" r:id="rId16" xr:uid="{DF584FDC-DE3A-4BDC-8E88-5ED7C38C9902}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Lancement de tous les cas de test
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbenjemi\Katalon Studio\ANEF_Eloignement_V1_Nawres\ANEF-Eloignement\ANEF_Eloignement_V1_Nawres\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA84FC0-A4B9-4B5F-AD8C-43BAE46205F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5A6109-B13E-4118-9E36-C7C8663D2334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3345,10 +3345,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}">
   <dimension ref="A1:FS173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AH1" sqref="AH1"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3700,7 +3700,7 @@
         <v>658</v>
       </c>
       <c r="E2" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F2" s="106">
         <v>7503182088</v>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="AI2" s="104"/>
       <c r="AJ2" s="104" t="s">
-        <v>632</v>
+        <v>221</v>
       </c>
       <c r="AK2" s="104" t="s">
         <v>685</v>
@@ -3935,10 +3935,10 @@
         <v>658</v>
       </c>
       <c r="E3" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F3" s="106">
-        <v>7503182266</v>
+        <v>7503182088</v>
       </c>
       <c r="G3" s="106" t="s">
         <v>615</v>
@@ -4162,10 +4162,10 @@
         <v>658</v>
       </c>
       <c r="E4" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F4" s="106">
-        <v>7503182266</v>
+        <v>7503182088</v>
       </c>
       <c r="G4" s="106" t="s">
         <v>615</v>
@@ -4397,7 +4397,7 @@
         <v>658</v>
       </c>
       <c r="E5" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F5" s="106">
         <v>7503182266</v>
@@ -4465,14 +4465,14 @@
       <c r="AG5" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="AH5" s="11" t="s">
+      <c r="AH5" s="104" t="s">
         <v>632</v>
       </c>
       <c r="AI5" s="104" t="s">
         <v>687</v>
       </c>
       <c r="AJ5" s="104" t="s">
-        <v>632</v>
+        <v>221</v>
       </c>
       <c r="AK5" s="104" t="s">
         <v>686</v>
@@ -4670,7 +4670,7 @@
       <c r="U6" s="84"/>
       <c r="V6" s="84"/>
       <c r="W6" s="84" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="X6" s="113" t="s">
         <v>662</v>
@@ -4841,7 +4841,7 @@
         <v>187</v>
       </c>
       <c r="E7" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F7" s="106">
         <v>7703056080</v>
@@ -5042,7 +5042,7 @@
         <v>658</v>
       </c>
       <c r="E8" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F8" s="106">
         <v>7503182092</v>
@@ -5239,7 +5239,7 @@
         <v>187</v>
       </c>
       <c r="E9" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F9" s="106">
         <v>7703056080</v>
@@ -5635,7 +5635,7 @@
         <v>658</v>
       </c>
       <c r="E11" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F11" s="106">
         <v>7503181980</v>
@@ -6222,7 +6222,7 @@
         <v>658</v>
       </c>
       <c r="E14" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F14" s="106">
         <v>7503181980</v>
@@ -6423,7 +6423,7 @@
         <v>658</v>
       </c>
       <c r="E15" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F15" s="106">
         <v>7503181980</v>
@@ -6624,7 +6624,7 @@
         <v>658</v>
       </c>
       <c r="E16" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F16" s="106">
         <v>7503181980</v>
@@ -7020,7 +7020,7 @@
         <v>187</v>
       </c>
       <c r="E18" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F18" s="106">
         <v>7703056080</v>

</xml_diff>

<commit_message>
adaptation mesures d'execution OQTF/REMISE SCHENGEN / TRANSFERT DUBLIN/ SIS
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbenjemi\Katalon Studio\ANEF_Eloignement_V1_Nawres\ANEF-Eloignement\ANEF_Eloignement_V1_Nawres\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6649D55-D94F-4570-8F64-AD60C9D3DBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D538AB59-496F-41BA-9A81-8FFBEBE6ACF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="prénom pour JDD" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$FS$153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$FS$156</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="697">
   <si>
     <t>URL_ANEFdevfenv5</t>
   </si>
@@ -2126,6 +2126,18 @@
   </si>
   <si>
     <t>AjouterRecoursContentieux</t>
+  </si>
+  <si>
+    <t>L. 731-2</t>
+  </si>
+  <si>
+    <t>AjouterICTF</t>
+  </si>
+  <si>
+    <t>L. 751-2</t>
+  </si>
+  <si>
+    <t>L. 751-6</t>
   </si>
 </sst>
 </file>
@@ -2607,7 +2619,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3030,6 +3042,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3343,12 +3361,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}">
-  <dimension ref="A1:FS173"/>
+  <dimension ref="A1:FS176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AH1" sqref="AH1"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3556,7 +3574,9 @@
       <c r="AR1" s="23" t="s">
         <v>692</v>
       </c>
-      <c r="AS1" s="13"/>
+      <c r="AS1" s="13" t="s">
+        <v>694</v>
+      </c>
       <c r="AT1" s="13"/>
       <c r="AU1" s="13"/>
       <c r="AV1" s="23"/>
@@ -4673,7 +4693,7 @@
         <v>645</v>
       </c>
       <c r="X6" s="113" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="Y6" s="104" t="s">
         <v>82</v>
@@ -4683,11 +4703,15 @@
       <c r="AB6" s="73"/>
       <c r="AC6" s="28"/>
       <c r="AD6" s="2"/>
-      <c r="AE6" s="28"/>
+      <c r="AE6" s="115" t="s">
+        <v>221</v>
+      </c>
       <c r="AF6" s="28"/>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="11"/>
+      <c r="AG6" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="AH6" s="104"/>
+      <c r="AI6" s="104"/>
       <c r="AJ6" s="11"/>
       <c r="AK6" s="11"/>
       <c r="AL6" s="11"/>
@@ -4702,7 +4726,9 @@
       <c r="AQ6" s="116" t="s">
         <v>632</v>
       </c>
-      <c r="AR6" s="12"/>
+      <c r="AR6" s="147" t="s">
+        <v>632</v>
+      </c>
       <c r="AS6" s="11"/>
       <c r="AT6" s="28"/>
       <c r="AU6" s="28"/>
@@ -4832,19 +4858,19 @@
         <v>74</v>
       </c>
       <c r="B7" s="104" t="s">
-        <v>76</v>
+        <v>599</v>
       </c>
       <c r="C7" s="105" t="s">
-        <v>631</v>
+        <v>644</v>
       </c>
       <c r="D7" s="105" t="s">
-        <v>187</v>
+        <v>658</v>
       </c>
       <c r="E7" s="106" t="s">
         <v>609</v>
       </c>
       <c r="F7" s="106">
-        <v>7703056113</v>
+        <v>7503182093</v>
       </c>
       <c r="G7" s="106" t="s">
         <v>625</v>
@@ -4882,9 +4908,15 @@
       <c r="T7" s="84"/>
       <c r="U7" s="84"/>
       <c r="V7" s="84"/>
-      <c r="W7" s="84"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="11"/>
+      <c r="W7" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X7" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y7" s="104" t="s">
+        <v>693</v>
+      </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="73"/>
@@ -4900,10 +4932,18 @@
       <c r="AL7" s="11"/>
       <c r="AM7" s="11"/>
       <c r="AN7" s="11"/>
-      <c r="AO7" s="11"/>
-      <c r="AP7" s="11"/>
-      <c r="AQ7" s="14"/>
-      <c r="AR7" s="12"/>
+      <c r="AO7" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AP7" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AQ7" s="116" t="s">
+        <v>632</v>
+      </c>
+      <c r="AR7" s="147" t="s">
+        <v>632</v>
+      </c>
       <c r="AS7" s="11"/>
       <c r="AT7" s="28"/>
       <c r="AU7" s="28"/>
@@ -5028,7 +5068,7 @@
       <c r="FO7" s="29"/>
       <c r="FP7" s="78"/>
     </row>
-    <row r="8" spans="1:175" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:175" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
@@ -5045,7 +5085,7 @@
         <v>609</v>
       </c>
       <c r="F8" s="106">
-        <v>7503182092</v>
+        <v>7503182093</v>
       </c>
       <c r="G8" s="106" t="s">
         <v>625</v>
@@ -5060,18 +5100,22 @@
         <v>617</v>
       </c>
       <c r="K8" s="106" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="L8" s="106" t="s">
-        <v>628</v>
+        <v>62</v>
       </c>
       <c r="M8" s="106" t="s">
-        <v>639</v>
+        <v>141</v>
       </c>
       <c r="N8" s="106"/>
       <c r="O8" s="106"/>
-      <c r="P8" s="106"/>
-      <c r="Q8" s="106"/>
+      <c r="P8" s="106" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q8" s="106" t="s">
+        <v>641</v>
+      </c>
       <c r="R8" s="106"/>
       <c r="S8" s="84" t="s">
         <v>194</v>
@@ -5079,9 +5123,15 @@
       <c r="T8" s="84"/>
       <c r="U8" s="84"/>
       <c r="V8" s="84"/>
-      <c r="W8" s="84"/>
-      <c r="X8" s="28"/>
-      <c r="Y8" s="11"/>
+      <c r="W8" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X8" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y8" s="104" t="s">
+        <v>693</v>
+      </c>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="73"/>
@@ -5092,15 +5142,33 @@
       <c r="AG8" s="2"/>
       <c r="AH8" s="11"/>
       <c r="AI8" s="11"/>
-      <c r="AJ8" s="11"/>
-      <c r="AK8" s="11"/>
-      <c r="AL8" s="11"/>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="11"/>
-      <c r="AO8" s="11"/>
-      <c r="AP8" s="11"/>
-      <c r="AQ8" s="14"/>
-      <c r="AR8" s="12"/>
+      <c r="AJ8" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AK8" s="104" t="s">
+        <v>686</v>
+      </c>
+      <c r="AL8" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM8" s="104" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN8" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AO8" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AP8" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AQ8" s="116" t="s">
+        <v>632</v>
+      </c>
+      <c r="AR8" s="147" t="s">
+        <v>221</v>
+      </c>
       <c r="AS8" s="11"/>
       <c r="AT8" s="28"/>
       <c r="AU8" s="28"/>
@@ -5225,24 +5293,24 @@
       <c r="FO8" s="29"/>
       <c r="FP8" s="78"/>
     </row>
-    <row r="9" spans="1:175" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:175" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B9" s="104" t="s">
-        <v>76</v>
+        <v>599</v>
       </c>
       <c r="C9" s="105" t="s">
-        <v>631</v>
+        <v>644</v>
       </c>
       <c r="D9" s="105" t="s">
-        <v>187</v>
+        <v>658</v>
       </c>
       <c r="E9" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F9" s="106">
-        <v>7703056113</v>
+        <v>7503182092</v>
       </c>
       <c r="G9" s="106" t="s">
         <v>625</v>
@@ -5257,50 +5325,70 @@
         <v>617</v>
       </c>
       <c r="K9" s="106" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="L9" s="106" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="M9" s="106" t="s">
-        <v>597</v>
+        <v>639</v>
       </c>
       <c r="N9" s="106"/>
       <c r="O9" s="106"/>
       <c r="P9" s="106"/>
       <c r="Q9" s="106"/>
-      <c r="R9" s="106" t="s">
-        <v>293</v>
-      </c>
+      <c r="R9" s="106"/>
       <c r="S9" s="84" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T9" s="84"/>
       <c r="U9" s="84"/>
       <c r="V9" s="84"/>
-      <c r="W9" s="84"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="11"/>
+      <c r="W9" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X9" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y9" s="104"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="73"/>
-      <c r="AC9" s="28"/>
+      <c r="AC9" s="115" t="s">
+        <v>632</v>
+      </c>
       <c r="AD9" s="2"/>
       <c r="AE9" s="28"/>
       <c r="AF9" s="28"/>
       <c r="AG9" s="2"/>
-      <c r="AH9" s="11"/>
-      <c r="AI9" s="11"/>
-      <c r="AJ9" s="11"/>
-      <c r="AK9" s="11"/>
-      <c r="AL9" s="11"/>
-      <c r="AM9" s="11"/>
-      <c r="AN9" s="11"/>
+      <c r="AH9" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI9" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ9" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AK9" s="104" t="s">
+        <v>686</v>
+      </c>
+      <c r="AL9" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM9" s="104" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN9" s="104" t="s">
+        <v>221</v>
+      </c>
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
       <c r="AQ9" s="14"/>
       <c r="AR9" s="12"/>
-      <c r="AS9" s="11"/>
+      <c r="AS9" s="104" t="s">
+        <v>632</v>
+      </c>
       <c r="AT9" s="28"/>
       <c r="AU9" s="28"/>
       <c r="AV9" s="2"/>
@@ -5424,82 +5512,104 @@
       <c r="FO9" s="29"/>
       <c r="FP9" s="78"/>
     </row>
-    <row r="10" spans="1:175" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:175" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B10" s="104" t="s">
-        <v>76</v>
+        <v>599</v>
       </c>
       <c r="C10" s="105" t="s">
-        <v>631</v>
+        <v>644</v>
       </c>
       <c r="D10" s="105" t="s">
-        <v>187</v>
+        <v>658</v>
       </c>
       <c r="E10" s="106" t="s">
         <v>609</v>
       </c>
       <c r="F10" s="106">
-        <v>7703056113</v>
+        <v>7503182092</v>
       </c>
       <c r="G10" s="106" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="H10" s="106">
-        <v>1994</v>
+        <v>1997</v>
       </c>
       <c r="I10" s="106" t="s">
         <v>192</v>
       </c>
       <c r="J10" s="106" t="s">
-        <v>645</v>
+        <v>617</v>
       </c>
       <c r="K10" s="106" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="L10" s="106" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="M10" s="106" t="s">
-        <v>597</v>
+        <v>639</v>
       </c>
       <c r="N10" s="106"/>
       <c r="O10" s="106"/>
       <c r="P10" s="106"/>
       <c r="Q10" s="106"/>
-      <c r="R10" s="106" t="s">
-        <v>294</v>
-      </c>
+      <c r="R10" s="106"/>
       <c r="S10" s="84" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T10" s="84"/>
       <c r="U10" s="84"/>
       <c r="V10" s="84"/>
-      <c r="W10" s="84"/>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="11"/>
+      <c r="W10" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X10" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y10" s="104"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="73"/>
-      <c r="AC10" s="28"/>
+      <c r="AC10" s="115" t="s">
+        <v>632</v>
+      </c>
       <c r="AD10" s="2"/>
       <c r="AE10" s="28"/>
       <c r="AF10" s="28"/>
       <c r="AG10" s="2"/>
-      <c r="AH10" s="11"/>
-      <c r="AI10" s="11"/>
-      <c r="AJ10" s="11"/>
-      <c r="AK10" s="11"/>
-      <c r="AL10" s="11"/>
-      <c r="AM10" s="11"/>
-      <c r="AN10" s="11"/>
+      <c r="AH10" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI10" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ10" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AK10" s="104" t="s">
+        <v>686</v>
+      </c>
+      <c r="AL10" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM10" s="104" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN10" s="104" t="s">
+        <v>221</v>
+      </c>
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
       <c r="AQ10" s="14"/>
-      <c r="AR10" s="12"/>
-      <c r="AS10" s="11"/>
+      <c r="AR10" s="147" t="s">
+        <v>632</v>
+      </c>
+      <c r="AS10" s="104" t="s">
+        <v>632</v>
+      </c>
       <c r="AT10" s="28"/>
       <c r="AU10" s="28"/>
       <c r="AV10" s="2"/>
@@ -5623,7 +5733,7 @@
       <c r="FO10" s="29"/>
       <c r="FP10" s="78"/>
     </row>
-    <row r="11" spans="1:175" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:175" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -5640,62 +5750,84 @@
         <v>609</v>
       </c>
       <c r="F11" s="106">
-        <v>7503181980</v>
+        <v>7503182092</v>
       </c>
       <c r="G11" s="106" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="H11" s="106">
-        <v>1994</v>
+        <v>1997</v>
       </c>
       <c r="I11" s="106" t="s">
         <v>192</v>
       </c>
       <c r="J11" s="106" t="s">
-        <v>645</v>
+        <v>617</v>
       </c>
       <c r="K11" s="106" t="s">
         <v>620</v>
       </c>
       <c r="L11" s="106" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="M11" s="106" t="s">
-        <v>637</v>
+        <v>597</v>
       </c>
       <c r="N11" s="106"/>
       <c r="O11" s="106"/>
       <c r="P11" s="106"/>
       <c r="Q11" s="106"/>
-      <c r="R11" s="106"/>
+      <c r="R11" s="106" t="s">
+        <v>293</v>
+      </c>
       <c r="S11" s="84" t="s">
         <v>195</v>
       </c>
       <c r="T11" s="84"/>
       <c r="U11" s="84"/>
       <c r="V11" s="84"/>
-      <c r="W11" s="84"/>
-      <c r="X11" s="28"/>
+      <c r="W11" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X11" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y11" s="11"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="73"/>
-      <c r="AC11" s="28"/>
+      <c r="AC11" s="115" t="s">
+        <v>632</v>
+      </c>
       <c r="AD11" s="2"/>
       <c r="AE11" s="28"/>
       <c r="AF11" s="28"/>
       <c r="AG11" s="2"/>
-      <c r="AH11" s="11"/>
-      <c r="AI11" s="11"/>
-      <c r="AJ11" s="11"/>
-      <c r="AK11" s="11"/>
-      <c r="AL11" s="11"/>
-      <c r="AM11" s="11"/>
+      <c r="AH11" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI11" s="104" t="s">
+        <v>695</v>
+      </c>
+      <c r="AJ11" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AK11" s="104" t="s">
+        <v>686</v>
+      </c>
+      <c r="AL11" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM11" s="104" t="s">
+        <v>308</v>
+      </c>
       <c r="AN11" s="11"/>
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
       <c r="AQ11" s="14"/>
-      <c r="AR11" s="12"/>
+      <c r="AR11" s="147" t="s">
+        <v>632</v>
+      </c>
       <c r="AS11" s="11"/>
       <c r="AT11" s="28"/>
       <c r="AU11" s="28"/>
@@ -5820,24 +5952,24 @@
       <c r="FO11" s="29"/>
       <c r="FP11" s="78"/>
     </row>
-    <row r="12" spans="1:175" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:175" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B12" s="104" t="s">
-        <v>76</v>
+        <v>599</v>
       </c>
       <c r="C12" s="105" t="s">
-        <v>631</v>
+        <v>644</v>
       </c>
       <c r="D12" s="105" t="s">
-        <v>187</v>
+        <v>658</v>
       </c>
       <c r="E12" s="106" t="s">
         <v>609</v>
       </c>
       <c r="F12" s="106">
-        <v>7703056113</v>
+        <v>7503182091</v>
       </c>
       <c r="G12" s="106" t="s">
         <v>615</v>
@@ -5852,39 +5984,55 @@
         <v>645</v>
       </c>
       <c r="K12" s="106" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="L12" s="106" t="s">
-        <v>66</v>
+        <v>629</v>
       </c>
       <c r="M12" s="106" t="s">
-        <v>335</v>
+        <v>597</v>
       </c>
       <c r="N12" s="106"/>
       <c r="O12" s="106"/>
       <c r="P12" s="106"/>
       <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
+      <c r="R12" s="106" t="s">
+        <v>294</v>
+      </c>
       <c r="S12" s="84" t="s">
         <v>195</v>
       </c>
       <c r="T12" s="84"/>
       <c r="U12" s="84"/>
       <c r="V12" s="84"/>
-      <c r="W12" s="84"/>
-      <c r="X12" s="28"/>
+      <c r="W12" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X12" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y12" s="11"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="73"/>
-      <c r="AC12" s="28"/>
+      <c r="AC12" s="115" t="s">
+        <v>221</v>
+      </c>
       <c r="AD12" s="2"/>
       <c r="AE12" s="28"/>
       <c r="AF12" s="28"/>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="11"/>
-      <c r="AI12" s="11"/>
-      <c r="AJ12" s="11"/>
+      <c r="AG12" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="AH12" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI12" s="104" t="s">
+        <v>696</v>
+      </c>
+      <c r="AJ12" s="104" t="s">
+        <v>221</v>
+      </c>
       <c r="AK12" s="11"/>
       <c r="AL12" s="11"/>
       <c r="AM12" s="11"/>
@@ -5892,7 +6040,9 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
       <c r="AQ12" s="14"/>
-      <c r="AR12" s="12"/>
+      <c r="AR12" s="147" t="s">
+        <v>632</v>
+      </c>
       <c r="AS12" s="11"/>
       <c r="AT12" s="28"/>
       <c r="AU12" s="28"/>
@@ -6017,24 +6167,24 @@
       <c r="FO12" s="29"/>
       <c r="FP12" s="78"/>
     </row>
-    <row r="13" spans="1:175" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:175" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B13" s="104" t="s">
-        <v>76</v>
+        <v>599</v>
       </c>
       <c r="C13" s="105" t="s">
-        <v>631</v>
+        <v>644</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>187</v>
+        <v>658</v>
       </c>
       <c r="E13" s="106" t="s">
         <v>609</v>
       </c>
       <c r="F13" s="106">
-        <v>7703056113</v>
+        <v>7503182091</v>
       </c>
       <c r="G13" s="106" t="s">
         <v>615</v>
@@ -6049,13 +6199,13 @@
         <v>645</v>
       </c>
       <c r="K13" s="106" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="L13" s="106" t="s">
-        <v>66</v>
+        <v>630</v>
       </c>
       <c r="M13" s="106" t="s">
-        <v>335</v>
+        <v>637</v>
       </c>
       <c r="N13" s="106"/>
       <c r="O13" s="106"/>
@@ -6063,33 +6213,54 @@
       <c r="Q13" s="106"/>
       <c r="R13" s="106"/>
       <c r="S13" s="84" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="T13" s="84"/>
       <c r="U13" s="84"/>
       <c r="V13" s="84"/>
-      <c r="W13" s="84"/>
-      <c r="X13" s="28"/>
+      <c r="W13" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X13" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y13" s="11"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="73"/>
-      <c r="AC13" s="28"/>
-      <c r="AD13" s="2"/>
+      <c r="AC13" s="115" t="s">
+        <v>632</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>3</v>
+      </c>
       <c r="AE13" s="28"/>
       <c r="AF13" s="28"/>
       <c r="AG13" s="2"/>
-      <c r="AH13" s="11"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="11"/>
-      <c r="AK13" s="11"/>
-      <c r="AL13" s="11"/>
-      <c r="AM13" s="11"/>
-      <c r="AN13" s="11"/>
+      <c r="AH13" s="11" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI13" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ13" s="11" t="s">
+        <v>632</v>
+      </c>
+      <c r="AK13" s="11" t="s">
+        <v>686</v>
+      </c>
+      <c r="AL13" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM13" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN13" s="11" t="s">
+        <v>632</v>
+      </c>
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
       <c r="AQ13" s="14"/>
-      <c r="AR13" s="12"/>
       <c r="AS13" s="11"/>
       <c r="AT13" s="28"/>
       <c r="AU13" s="28"/>
@@ -6214,7 +6385,7 @@
       <c r="FO13" s="29"/>
       <c r="FP13" s="78"/>
     </row>
-    <row r="14" spans="1:175" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:175" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>74</v>
       </c>
@@ -6231,7 +6402,7 @@
         <v>609</v>
       </c>
       <c r="F14" s="106">
-        <v>7503182086</v>
+        <v>7503182091</v>
       </c>
       <c r="G14" s="106" t="s">
         <v>615</v>
@@ -6243,54 +6414,74 @@
         <v>192</v>
       </c>
       <c r="J14" s="106" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="K14" s="106" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="L14" s="106" t="s">
-        <v>67</v>
-      </c>
-      <c r="M14" s="106"/>
+        <v>630</v>
+      </c>
+      <c r="M14" s="106" t="s">
+        <v>637</v>
+      </c>
       <c r="N14" s="106"/>
       <c r="O14" s="106"/>
       <c r="P14" s="106"/>
       <c r="Q14" s="106"/>
       <c r="R14" s="106"/>
       <c r="S14" s="84" t="s">
-        <v>194</v>
-      </c>
-      <c r="T14" s="84" t="s">
-        <v>657</v>
-      </c>
-      <c r="U14" s="84" t="s">
-        <v>651</v>
-      </c>
-      <c r="V14" s="84" t="s">
-        <v>654</v>
-      </c>
-      <c r="W14" s="84"/>
-      <c r="X14" s="28"/>
+        <v>195</v>
+      </c>
+      <c r="T14" s="84"/>
+      <c r="U14" s="84"/>
+      <c r="V14" s="84"/>
+      <c r="W14" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X14" s="113" t="s">
+        <v>663</v>
+      </c>
       <c r="Y14" s="11"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="73"/>
-      <c r="AC14" s="28"/>
-      <c r="AD14" s="2"/>
+      <c r="AC14" s="115" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>3</v>
+      </c>
       <c r="AE14" s="28"/>
       <c r="AF14" s="28"/>
       <c r="AG14" s="2"/>
-      <c r="AH14" s="11"/>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11"/>
-      <c r="AK14" s="11"/>
-      <c r="AL14" s="11"/>
-      <c r="AM14" s="11"/>
-      <c r="AN14" s="11"/>
+      <c r="AH14" s="11" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI14" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ14" s="11" t="s">
+        <v>632</v>
+      </c>
+      <c r="AK14" s="11" t="s">
+        <v>686</v>
+      </c>
+      <c r="AL14" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM14" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN14" s="11" t="s">
+        <v>632</v>
+      </c>
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
       <c r="AQ14" s="14"/>
-      <c r="AR14" s="12"/>
+      <c r="AR14" s="12" t="s">
+        <v>632</v>
+      </c>
       <c r="AS14" s="11"/>
       <c r="AT14" s="28"/>
       <c r="AU14" s="28"/>
@@ -6415,24 +6606,24 @@
       <c r="FO14" s="29"/>
       <c r="FP14" s="78"/>
     </row>
-    <row r="15" spans="1:175" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:175" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B15" s="104" t="s">
-        <v>599</v>
+        <v>76</v>
       </c>
       <c r="C15" s="105" t="s">
-        <v>644</v>
+        <v>631</v>
       </c>
       <c r="D15" s="105" t="s">
-        <v>658</v>
+        <v>187</v>
       </c>
       <c r="E15" s="106" t="s">
         <v>609</v>
       </c>
       <c r="F15" s="106">
-        <v>7503182086</v>
+        <v>7703056113</v>
       </c>
       <c r="G15" s="106" t="s">
         <v>615</v>
@@ -6444,32 +6635,28 @@
         <v>192</v>
       </c>
       <c r="J15" s="106" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="K15" s="106" t="s">
         <v>622</v>
       </c>
       <c r="L15" s="106" t="s">
-        <v>67</v>
-      </c>
-      <c r="M15" s="106"/>
+        <v>66</v>
+      </c>
+      <c r="M15" s="106" t="s">
+        <v>335</v>
+      </c>
       <c r="N15" s="106"/>
       <c r="O15" s="106"/>
       <c r="P15" s="106"/>
       <c r="Q15" s="106"/>
       <c r="R15" s="106"/>
       <c r="S15" s="84" t="s">
-        <v>194</v>
-      </c>
-      <c r="T15" s="84" t="s">
-        <v>657</v>
-      </c>
-      <c r="U15" s="84" t="s">
-        <v>652</v>
-      </c>
-      <c r="V15" s="84" t="s">
-        <v>655</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="T15" s="84"/>
+      <c r="U15" s="84"/>
+      <c r="V15" s="84"/>
       <c r="W15" s="84"/>
       <c r="X15" s="28"/>
       <c r="Y15" s="11"/>
@@ -6616,24 +6803,24 @@
       <c r="FO15" s="29"/>
       <c r="FP15" s="78"/>
     </row>
-    <row r="16" spans="1:175" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:175" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B16" s="104" t="s">
-        <v>599</v>
+        <v>76</v>
       </c>
       <c r="C16" s="105" t="s">
-        <v>644</v>
+        <v>631</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>658</v>
+        <v>187</v>
       </c>
       <c r="E16" s="106" t="s">
         <v>609</v>
       </c>
       <c r="F16" s="106">
-        <v>7503182086</v>
+        <v>7703056113</v>
       </c>
       <c r="G16" s="106" t="s">
         <v>615</v>
@@ -6645,15 +6832,17 @@
         <v>192</v>
       </c>
       <c r="J16" s="106" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="K16" s="106" t="s">
         <v>622</v>
       </c>
       <c r="L16" s="106" t="s">
-        <v>67</v>
-      </c>
-      <c r="M16" s="106"/>
+        <v>66</v>
+      </c>
+      <c r="M16" s="106" t="s">
+        <v>335</v>
+      </c>
       <c r="N16" s="106"/>
       <c r="O16" s="106"/>
       <c r="P16" s="106"/>
@@ -6662,13 +6851,9 @@
       <c r="S16" s="84" t="s">
         <v>194</v>
       </c>
-      <c r="T16" s="84" t="s">
-        <v>656</v>
-      </c>
+      <c r="T16" s="84"/>
       <c r="U16" s="84"/>
-      <c r="V16" s="84" t="s">
-        <v>654</v>
-      </c>
+      <c r="V16" s="84"/>
       <c r="W16" s="84"/>
       <c r="X16" s="28"/>
       <c r="Y16" s="11"/>
@@ -6820,19 +7005,19 @@
         <v>74</v>
       </c>
       <c r="B17" s="104" t="s">
-        <v>76</v>
+        <v>599</v>
       </c>
       <c r="C17" s="105" t="s">
-        <v>631</v>
+        <v>644</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>187</v>
+        <v>658</v>
       </c>
       <c r="E17" s="106" t="s">
         <v>609</v>
       </c>
       <c r="F17" s="106">
-        <v>7703056113</v>
+        <v>7503182086</v>
       </c>
       <c r="G17" s="106" t="s">
         <v>615</v>
@@ -6862,9 +7047,11 @@
         <v>194</v>
       </c>
       <c r="T17" s="84" t="s">
-        <v>656</v>
-      </c>
-      <c r="U17" s="84"/>
+        <v>657</v>
+      </c>
+      <c r="U17" s="84" t="s">
+        <v>651</v>
+      </c>
       <c r="V17" s="84" t="s">
         <v>654</v>
       </c>
@@ -7014,24 +7201,24 @@
       <c r="FO17" s="29"/>
       <c r="FP17" s="78"/>
     </row>
-    <row r="18" spans="1:172" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:172" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="104" t="s">
-        <v>76</v>
+        <v>599</v>
       </c>
       <c r="C18" s="105" t="s">
-        <v>631</v>
+        <v>644</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>187</v>
+        <v>658</v>
       </c>
       <c r="E18" s="106" t="s">
         <v>609</v>
       </c>
       <c r="F18" s="106">
-        <v>7703056113</v>
+        <v>7503182086</v>
       </c>
       <c r="G18" s="106" t="s">
         <v>615</v>
@@ -7046,7 +7233,7 @@
         <v>649</v>
       </c>
       <c r="K18" s="106" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="L18" s="106" t="s">
         <v>67</v>
@@ -7058,14 +7245,16 @@
       <c r="Q18" s="106"/>
       <c r="R18" s="106"/>
       <c r="S18" s="84" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T18" s="84" t="s">
-        <v>656</v>
-      </c>
-      <c r="U18" s="84"/>
+        <v>657</v>
+      </c>
+      <c r="U18" s="84" t="s">
+        <v>652</v>
+      </c>
       <c r="V18" s="84" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="W18" s="84"/>
       <c r="X18" s="28"/>
@@ -7213,280 +7402,853 @@
       <c r="FO18" s="29"/>
       <c r="FP18" s="78"/>
     </row>
-    <row r="19" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="AG19"/>
-      <c r="AH19" s="37"/>
-      <c r="AI19" s="37"/>
-    </row>
-    <row r="20" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="AG20"/>
-      <c r="AH20" s="37"/>
-      <c r="AI20" s="37"/>
-    </row>
-    <row r="21" spans="1:172" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="141" t="s">
+    <row r="19" spans="1:172" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="104" t="s">
+        <v>599</v>
+      </c>
+      <c r="C19" s="105" t="s">
+        <v>644</v>
+      </c>
+      <c r="D19" s="105" t="s">
+        <v>658</v>
+      </c>
+      <c r="E19" s="106" t="s">
+        <v>609</v>
+      </c>
+      <c r="F19" s="106">
+        <v>7503182086</v>
+      </c>
+      <c r="G19" s="106" t="s">
+        <v>615</v>
+      </c>
+      <c r="H19" s="106">
+        <v>1994</v>
+      </c>
+      <c r="I19" s="106" t="s">
+        <v>192</v>
+      </c>
+      <c r="J19" s="106" t="s">
+        <v>649</v>
+      </c>
+      <c r="K19" s="106" t="s">
+        <v>622</v>
+      </c>
+      <c r="L19" s="106" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" s="106"/>
+      <c r="N19" s="106"/>
+      <c r="O19" s="106"/>
+      <c r="P19" s="106"/>
+      <c r="Q19" s="106"/>
+      <c r="R19" s="106"/>
+      <c r="S19" s="84" t="s">
+        <v>194</v>
+      </c>
+      <c r="T19" s="84" t="s">
+        <v>656</v>
+      </c>
+      <c r="U19" s="84"/>
+      <c r="V19" s="84" t="s">
+        <v>654</v>
+      </c>
+      <c r="W19" s="84"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="73"/>
+      <c r="AC19" s="28"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="11"/>
+      <c r="AM19" s="11"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="11"/>
+      <c r="AP19" s="11"/>
+      <c r="AQ19" s="14"/>
+      <c r="AR19" s="12"/>
+      <c r="AS19" s="11"/>
+      <c r="AT19" s="28"/>
+      <c r="AU19" s="28"/>
+      <c r="AV19" s="2"/>
+      <c r="AW19" s="2"/>
+      <c r="AX19" s="2"/>
+      <c r="AY19" s="55"/>
+      <c r="AZ19" s="42"/>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="2"/>
+      <c r="BD19" s="2"/>
+      <c r="BE19" s="2"/>
+      <c r="BF19" s="5"/>
+      <c r="BG19" s="5"/>
+      <c r="BH19" s="74"/>
+      <c r="BI19" s="74"/>
+      <c r="BJ19" s="74"/>
+      <c r="BK19" s="74"/>
+      <c r="BL19" s="74"/>
+      <c r="BM19" s="74"/>
+      <c r="BN19" s="74"/>
+      <c r="BO19" s="74"/>
+      <c r="BP19" s="74"/>
+      <c r="BQ19" s="74"/>
+      <c r="BR19" s="74"/>
+      <c r="BS19" s="75"/>
+      <c r="BT19" s="74"/>
+      <c r="BU19" s="74"/>
+      <c r="BV19" s="74"/>
+      <c r="BW19" s="74"/>
+      <c r="BX19" s="74"/>
+      <c r="BY19" s="74"/>
+      <c r="BZ19" s="74"/>
+      <c r="CA19" s="74"/>
+      <c r="CB19" s="74"/>
+      <c r="CC19" s="74"/>
+      <c r="CD19" s="74"/>
+      <c r="CE19" s="74"/>
+      <c r="CF19" s="74"/>
+      <c r="CG19" s="76"/>
+      <c r="CH19" s="76"/>
+      <c r="CI19" s="74"/>
+      <c r="CJ19" s="76"/>
+      <c r="CK19" s="76"/>
+      <c r="CL19" s="74"/>
+      <c r="CM19" s="74"/>
+      <c r="CN19" s="74"/>
+      <c r="CO19" s="74"/>
+      <c r="CP19" s="74"/>
+      <c r="CQ19" s="74"/>
+      <c r="CR19" s="76"/>
+      <c r="CS19" s="76"/>
+      <c r="CT19" s="74"/>
+      <c r="CU19" s="79"/>
+      <c r="CV19" s="74"/>
+      <c r="CW19" s="74"/>
+      <c r="CX19" s="74"/>
+      <c r="CY19" s="76"/>
+      <c r="CZ19" s="76"/>
+      <c r="DA19" s="74"/>
+      <c r="DB19" s="74"/>
+      <c r="DC19" s="74"/>
+      <c r="DD19" s="74"/>
+      <c r="DE19" s="74"/>
+      <c r="DF19" s="74"/>
+      <c r="DG19" s="74"/>
+      <c r="DH19" s="74"/>
+      <c r="DI19" s="74"/>
+      <c r="DJ19" s="74"/>
+      <c r="DK19" s="74"/>
+      <c r="DL19" s="74"/>
+      <c r="DM19" s="76"/>
+      <c r="DN19" s="76"/>
+      <c r="DO19" s="76"/>
+      <c r="DP19" s="76"/>
+      <c r="DQ19" s="76"/>
+      <c r="DR19" s="76"/>
+      <c r="DS19" s="76"/>
+      <c r="DT19" s="76"/>
+      <c r="DU19" s="76"/>
+      <c r="DV19" s="76"/>
+      <c r="DW19" s="74"/>
+      <c r="DX19" s="74"/>
+      <c r="DY19" s="74"/>
+      <c r="DZ19" s="74"/>
+      <c r="EA19" s="74"/>
+      <c r="EB19" s="74"/>
+      <c r="EC19" s="76"/>
+      <c r="ED19" s="76"/>
+      <c r="EE19" s="74"/>
+      <c r="EF19" s="2"/>
+      <c r="EG19" s="2"/>
+      <c r="EH19" s="2"/>
+      <c r="EI19" s="2"/>
+      <c r="EJ19" s="2"/>
+      <c r="EK19" s="5"/>
+      <c r="EL19" s="5"/>
+      <c r="EM19" s="5"/>
+      <c r="EN19" s="5"/>
+      <c r="EO19" s="5"/>
+      <c r="EP19" s="5"/>
+      <c r="EQ19" s="5"/>
+      <c r="ER19" s="5"/>
+      <c r="ES19" s="5"/>
+      <c r="ET19" s="5"/>
+      <c r="EU19" s="5"/>
+      <c r="EV19" s="5"/>
+      <c r="EW19" s="5"/>
+      <c r="EX19" s="5"/>
+      <c r="EY19" s="5"/>
+      <c r="EZ19" s="5"/>
+      <c r="FA19" s="5"/>
+      <c r="FB19" s="5"/>
+      <c r="FC19" s="5"/>
+      <c r="FD19" s="5"/>
+      <c r="FH19" s="56"/>
+      <c r="FK19" s="29"/>
+      <c r="FL19" s="29"/>
+      <c r="FM19" s="29"/>
+      <c r="FN19" s="29"/>
+      <c r="FO19" s="29"/>
+      <c r="FP19" s="78"/>
+    </row>
+    <row r="20" spans="1:172" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="105" t="s">
+        <v>631</v>
+      </c>
+      <c r="D20" s="105" t="s">
+        <v>187</v>
+      </c>
+      <c r="E20" s="106" t="s">
+        <v>609</v>
+      </c>
+      <c r="F20" s="106">
+        <v>7703056113</v>
+      </c>
+      <c r="G20" s="106" t="s">
+        <v>615</v>
+      </c>
+      <c r="H20" s="106">
+        <v>1994</v>
+      </c>
+      <c r="I20" s="106" t="s">
+        <v>192</v>
+      </c>
+      <c r="J20" s="106" t="s">
+        <v>649</v>
+      </c>
+      <c r="K20" s="106" t="s">
+        <v>622</v>
+      </c>
+      <c r="L20" s="106" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" s="106"/>
+      <c r="N20" s="106"/>
+      <c r="O20" s="106"/>
+      <c r="P20" s="106"/>
+      <c r="Q20" s="106"/>
+      <c r="R20" s="106"/>
+      <c r="S20" s="84" t="s">
+        <v>194</v>
+      </c>
+      <c r="T20" s="84" t="s">
+        <v>656</v>
+      </c>
+      <c r="U20" s="84"/>
+      <c r="V20" s="84" t="s">
+        <v>654</v>
+      </c>
+      <c r="W20" s="84"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="73"/>
+      <c r="AC20" s="28"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="28"/>
+      <c r="AF20" s="28"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="11"/>
+      <c r="AI20" s="11"/>
+      <c r="AJ20" s="11"/>
+      <c r="AK20" s="11"/>
+      <c r="AL20" s="11"/>
+      <c r="AM20" s="11"/>
+      <c r="AN20" s="11"/>
+      <c r="AO20" s="11"/>
+      <c r="AP20" s="11"/>
+      <c r="AQ20" s="14"/>
+      <c r="AR20" s="12"/>
+      <c r="AS20" s="11"/>
+      <c r="AT20" s="28"/>
+      <c r="AU20" s="28"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+      <c r="AX20" s="2"/>
+      <c r="AY20" s="55"/>
+      <c r="AZ20" s="42"/>
+      <c r="BA20" s="2"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="2"/>
+      <c r="BD20" s="2"/>
+      <c r="BE20" s="2"/>
+      <c r="BF20" s="5"/>
+      <c r="BG20" s="5"/>
+      <c r="BH20" s="74"/>
+      <c r="BI20" s="74"/>
+      <c r="BJ20" s="74"/>
+      <c r="BK20" s="74"/>
+      <c r="BL20" s="74"/>
+      <c r="BM20" s="74"/>
+      <c r="BN20" s="74"/>
+      <c r="BO20" s="74"/>
+      <c r="BP20" s="74"/>
+      <c r="BQ20" s="74"/>
+      <c r="BR20" s="74"/>
+      <c r="BS20" s="75"/>
+      <c r="BT20" s="74"/>
+      <c r="BU20" s="74"/>
+      <c r="BV20" s="74"/>
+      <c r="BW20" s="74"/>
+      <c r="BX20" s="74"/>
+      <c r="BY20" s="74"/>
+      <c r="BZ20" s="74"/>
+      <c r="CA20" s="74"/>
+      <c r="CB20" s="74"/>
+      <c r="CC20" s="74"/>
+      <c r="CD20" s="74"/>
+      <c r="CE20" s="74"/>
+      <c r="CF20" s="74"/>
+      <c r="CG20" s="76"/>
+      <c r="CH20" s="76"/>
+      <c r="CI20" s="74"/>
+      <c r="CJ20" s="76"/>
+      <c r="CK20" s="76"/>
+      <c r="CL20" s="74"/>
+      <c r="CM20" s="74"/>
+      <c r="CN20" s="74"/>
+      <c r="CO20" s="74"/>
+      <c r="CP20" s="74"/>
+      <c r="CQ20" s="74"/>
+      <c r="CR20" s="76"/>
+      <c r="CS20" s="76"/>
+      <c r="CT20" s="74"/>
+      <c r="CU20" s="79"/>
+      <c r="CV20" s="74"/>
+      <c r="CW20" s="74"/>
+      <c r="CX20" s="74"/>
+      <c r="CY20" s="76"/>
+      <c r="CZ20" s="76"/>
+      <c r="DA20" s="74"/>
+      <c r="DB20" s="74"/>
+      <c r="DC20" s="74"/>
+      <c r="DD20" s="74"/>
+      <c r="DE20" s="74"/>
+      <c r="DF20" s="74"/>
+      <c r="DG20" s="74"/>
+      <c r="DH20" s="74"/>
+      <c r="DI20" s="74"/>
+      <c r="DJ20" s="74"/>
+      <c r="DK20" s="74"/>
+      <c r="DL20" s="74"/>
+      <c r="DM20" s="76"/>
+      <c r="DN20" s="76"/>
+      <c r="DO20" s="76"/>
+      <c r="DP20" s="76"/>
+      <c r="DQ20" s="76"/>
+      <c r="DR20" s="76"/>
+      <c r="DS20" s="76"/>
+      <c r="DT20" s="76"/>
+      <c r="DU20" s="76"/>
+      <c r="DV20" s="76"/>
+      <c r="DW20" s="74"/>
+      <c r="DX20" s="74"/>
+      <c r="DY20" s="74"/>
+      <c r="DZ20" s="74"/>
+      <c r="EA20" s="74"/>
+      <c r="EB20" s="74"/>
+      <c r="EC20" s="76"/>
+      <c r="ED20" s="76"/>
+      <c r="EE20" s="74"/>
+      <c r="EF20" s="2"/>
+      <c r="EG20" s="2"/>
+      <c r="EH20" s="2"/>
+      <c r="EI20" s="2"/>
+      <c r="EJ20" s="2"/>
+      <c r="EK20" s="5"/>
+      <c r="EL20" s="5"/>
+      <c r="EM20" s="5"/>
+      <c r="EN20" s="5"/>
+      <c r="EO20" s="5"/>
+      <c r="EP20" s="5"/>
+      <c r="EQ20" s="5"/>
+      <c r="ER20" s="5"/>
+      <c r="ES20" s="5"/>
+      <c r="ET20" s="5"/>
+      <c r="EU20" s="5"/>
+      <c r="EV20" s="5"/>
+      <c r="EW20" s="5"/>
+      <c r="EX20" s="5"/>
+      <c r="EY20" s="5"/>
+      <c r="EZ20" s="5"/>
+      <c r="FA20" s="5"/>
+      <c r="FB20" s="5"/>
+      <c r="FC20" s="5"/>
+      <c r="FD20" s="5"/>
+      <c r="FH20" s="56"/>
+      <c r="FK20" s="29"/>
+      <c r="FL20" s="29"/>
+      <c r="FM20" s="29"/>
+      <c r="FN20" s="29"/>
+      <c r="FO20" s="29"/>
+      <c r="FP20" s="78"/>
+    </row>
+    <row r="21" spans="1:172" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="105" t="s">
+        <v>631</v>
+      </c>
+      <c r="D21" s="105" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="106" t="s">
+        <v>609</v>
+      </c>
+      <c r="F21" s="106">
+        <v>7703056113</v>
+      </c>
+      <c r="G21" s="106" t="s">
+        <v>615</v>
+      </c>
+      <c r="H21" s="106">
+        <v>1994</v>
+      </c>
+      <c r="I21" s="106" t="s">
+        <v>192</v>
+      </c>
+      <c r="J21" s="106" t="s">
+        <v>649</v>
+      </c>
+      <c r="K21" s="106" t="s">
+        <v>620</v>
+      </c>
+      <c r="L21" s="106" t="s">
+        <v>67</v>
+      </c>
+      <c r="M21" s="106"/>
+      <c r="N21" s="106"/>
+      <c r="O21" s="106"/>
+      <c r="P21" s="106"/>
+      <c r="Q21" s="106"/>
+      <c r="R21" s="106"/>
+      <c r="S21" s="84" t="s">
+        <v>195</v>
+      </c>
+      <c r="T21" s="84" t="s">
+        <v>656</v>
+      </c>
+      <c r="U21" s="84"/>
+      <c r="V21" s="84" t="s">
+        <v>654</v>
+      </c>
+      <c r="W21" s="84"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="73"/>
+      <c r="AC21" s="28"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="28"/>
+      <c r="AF21" s="28"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="11"/>
+      <c r="AJ21" s="11"/>
+      <c r="AK21" s="11"/>
+      <c r="AL21" s="11"/>
+      <c r="AM21" s="11"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="11"/>
+      <c r="AP21" s="11"/>
+      <c r="AQ21" s="14"/>
+      <c r="AR21" s="12"/>
+      <c r="AS21" s="11"/>
+      <c r="AT21" s="28"/>
+      <c r="AU21" s="28"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+      <c r="AX21" s="2"/>
+      <c r="AY21" s="55"/>
+      <c r="AZ21" s="42"/>
+      <c r="BA21" s="2"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="2"/>
+      <c r="BD21" s="2"/>
+      <c r="BE21" s="2"/>
+      <c r="BF21" s="5"/>
+      <c r="BG21" s="5"/>
+      <c r="BH21" s="74"/>
+      <c r="BI21" s="74"/>
+      <c r="BJ21" s="74"/>
+      <c r="BK21" s="74"/>
+      <c r="BL21" s="74"/>
+      <c r="BM21" s="74"/>
+      <c r="BN21" s="74"/>
+      <c r="BO21" s="74"/>
+      <c r="BP21" s="74"/>
+      <c r="BQ21" s="74"/>
+      <c r="BR21" s="74"/>
+      <c r="BS21" s="75"/>
+      <c r="BT21" s="74"/>
+      <c r="BU21" s="74"/>
+      <c r="BV21" s="74"/>
+      <c r="BW21" s="74"/>
+      <c r="BX21" s="74"/>
+      <c r="BY21" s="74"/>
+      <c r="BZ21" s="74"/>
+      <c r="CA21" s="74"/>
+      <c r="CB21" s="74"/>
+      <c r="CC21" s="74"/>
+      <c r="CD21" s="74"/>
+      <c r="CE21" s="74"/>
+      <c r="CF21" s="74"/>
+      <c r="CG21" s="76"/>
+      <c r="CH21" s="76"/>
+      <c r="CI21" s="74"/>
+      <c r="CJ21" s="76"/>
+      <c r="CK21" s="76"/>
+      <c r="CL21" s="74"/>
+      <c r="CM21" s="74"/>
+      <c r="CN21" s="74"/>
+      <c r="CO21" s="74"/>
+      <c r="CP21" s="74"/>
+      <c r="CQ21" s="74"/>
+      <c r="CR21" s="76"/>
+      <c r="CS21" s="76"/>
+      <c r="CT21" s="74"/>
+      <c r="CU21" s="79"/>
+      <c r="CV21" s="74"/>
+      <c r="CW21" s="74"/>
+      <c r="CX21" s="74"/>
+      <c r="CY21" s="76"/>
+      <c r="CZ21" s="76"/>
+      <c r="DA21" s="74"/>
+      <c r="DB21" s="74"/>
+      <c r="DC21" s="74"/>
+      <c r="DD21" s="74"/>
+      <c r="DE21" s="74"/>
+      <c r="DF21" s="74"/>
+      <c r="DG21" s="74"/>
+      <c r="DH21" s="74"/>
+      <c r="DI21" s="74"/>
+      <c r="DJ21" s="74"/>
+      <c r="DK21" s="74"/>
+      <c r="DL21" s="74"/>
+      <c r="DM21" s="76"/>
+      <c r="DN21" s="76"/>
+      <c r="DO21" s="76"/>
+      <c r="DP21" s="76"/>
+      <c r="DQ21" s="76"/>
+      <c r="DR21" s="76"/>
+      <c r="DS21" s="76"/>
+      <c r="DT21" s="76"/>
+      <c r="DU21" s="76"/>
+      <c r="DV21" s="76"/>
+      <c r="DW21" s="74"/>
+      <c r="DX21" s="74"/>
+      <c r="DY21" s="74"/>
+      <c r="DZ21" s="74"/>
+      <c r="EA21" s="74"/>
+      <c r="EB21" s="74"/>
+      <c r="EC21" s="76"/>
+      <c r="ED21" s="76"/>
+      <c r="EE21" s="74"/>
+      <c r="EF21" s="2"/>
+      <c r="EG21" s="2"/>
+      <c r="EH21" s="2"/>
+      <c r="EI21" s="2"/>
+      <c r="EJ21" s="2"/>
+      <c r="EK21" s="5"/>
+      <c r="EL21" s="5"/>
+      <c r="EM21" s="5"/>
+      <c r="EN21" s="5"/>
+      <c r="EO21" s="5"/>
+      <c r="EP21" s="5"/>
+      <c r="EQ21" s="5"/>
+      <c r="ER21" s="5"/>
+      <c r="ES21" s="5"/>
+      <c r="ET21" s="5"/>
+      <c r="EU21" s="5"/>
+      <c r="EV21" s="5"/>
+      <c r="EW21" s="5"/>
+      <c r="EX21" s="5"/>
+      <c r="EY21" s="5"/>
+      <c r="EZ21" s="5"/>
+      <c r="FA21" s="5"/>
+      <c r="FB21" s="5"/>
+      <c r="FC21" s="5"/>
+      <c r="FD21" s="5"/>
+      <c r="FH21" s="56"/>
+      <c r="FK21" s="29"/>
+      <c r="FL21" s="29"/>
+      <c r="FM21" s="29"/>
+      <c r="FN21" s="29"/>
+      <c r="FO21" s="29"/>
+      <c r="FP21" s="78"/>
+    </row>
+    <row r="22" spans="1:172" x14ac:dyDescent="0.3">
+      <c r="AG22"/>
+      <c r="AH22" s="37"/>
+      <c r="AI22" s="37"/>
+    </row>
+    <row r="23" spans="1:172" x14ac:dyDescent="0.3">
+      <c r="AG23"/>
+      <c r="AH23" s="37"/>
+      <c r="AI23" s="37"/>
+    </row>
+    <row r="24" spans="1:172" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="141" t="s">
         <v>600</v>
       </c>
-      <c r="B21" s="142"/>
-      <c r="C21" s="142"/>
-      <c r="D21" s="142"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="81"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="81"/>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="81"/>
-      <c r="S21" s="81"/>
-      <c r="T21" s="81"/>
-      <c r="U21" s="81"/>
-      <c r="V21" s="81"/>
-      <c r="W21" s="81"/>
-    </row>
-    <row r="22" spans="1:172" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="143" t="s">
+      <c r="B24" s="142"/>
+      <c r="C24" s="142"/>
+      <c r="D24" s="142"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="81"/>
+      <c r="L24" s="81"/>
+      <c r="M24" s="81"/>
+      <c r="N24" s="81"/>
+      <c r="O24" s="81"/>
+      <c r="P24" s="81"/>
+      <c r="Q24" s="81"/>
+      <c r="R24" s="81"/>
+      <c r="S24" s="81"/>
+      <c r="T24" s="81"/>
+      <c r="U24" s="81"/>
+      <c r="V24" s="81"/>
+      <c r="W24" s="81"/>
+    </row>
+    <row r="25" spans="1:172" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="143" t="s">
         <v>601</v>
       </c>
-      <c r="B22" s="143"/>
-      <c r="C22" s="85" t="s">
+      <c r="B25" s="143"/>
+      <c r="C25" s="85" t="s">
         <v>602</v>
       </c>
-      <c r="D22" s="146"/>
-    </row>
-    <row r="23" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A23" s="144" t="s">
+      <c r="D25" s="146"/>
+    </row>
+    <row r="26" spans="1:172" x14ac:dyDescent="0.3">
+      <c r="A26" s="144" t="s">
         <v>218</v>
       </c>
-      <c r="B23" s="145"/>
-      <c r="C23" s="83" t="s">
+      <c r="B26" s="145"/>
+      <c r="C26" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="146"/>
-    </row>
-    <row r="24" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A24" s="124" t="s">
+      <c r="D26" s="146"/>
+    </row>
+    <row r="27" spans="1:172" x14ac:dyDescent="0.3">
+      <c r="A27" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="128"/>
-      <c r="C24" s="82" t="s">
+      <c r="B27" s="128"/>
+      <c r="C27" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="146"/>
-    </row>
-    <row r="25" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A25" s="124"/>
-      <c r="B25" s="128"/>
-      <c r="C25" s="82" t="s">
-        <v>599</v>
-      </c>
-      <c r="D25" s="146"/>
-    </row>
-    <row r="26" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A26" s="119" t="s">
-        <v>603</v>
-      </c>
-      <c r="B26" s="120"/>
-      <c r="C26" s="83" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="146"/>
-    </row>
-    <row r="27" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A27" s="119"/>
-      <c r="B27" s="120"/>
-      <c r="C27" s="83" t="s">
-        <v>604</v>
-      </c>
       <c r="D27" s="146"/>
     </row>
     <row r="28" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A28" s="124" t="s">
-        <v>605</v>
-      </c>
+      <c r="A28" s="124"/>
       <c r="B28" s="128"/>
       <c r="C28" s="82" t="s">
+        <v>599</v>
+      </c>
+      <c r="D28" s="146"/>
+    </row>
+    <row r="29" spans="1:172" x14ac:dyDescent="0.3">
+      <c r="A29" s="119" t="s">
+        <v>603</v>
+      </c>
+      <c r="B29" s="120"/>
+      <c r="C29" s="83" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="146"/>
+    </row>
+    <row r="30" spans="1:172" x14ac:dyDescent="0.3">
+      <c r="A30" s="119"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="83" t="s">
+        <v>604</v>
+      </c>
+      <c r="D30" s="146"/>
+    </row>
+    <row r="31" spans="1:172" x14ac:dyDescent="0.3">
+      <c r="A31" s="124" t="s">
+        <v>605</v>
+      </c>
+      <c r="B31" s="128"/>
+      <c r="C31" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="146"/>
-    </row>
-    <row r="29" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A29" s="124"/>
-      <c r="B29" s="128"/>
-      <c r="C29" s="82" t="s">
+      <c r="D31" s="146"/>
+    </row>
+    <row r="32" spans="1:172" x14ac:dyDescent="0.3">
+      <c r="A32" s="124"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="82" t="s">
         <v>606</v>
       </c>
-      <c r="D29" s="146"/>
-    </row>
-    <row r="30" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A30" s="119" t="s">
+      <c r="D32" s="146"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="119" t="s">
         <v>607</v>
       </c>
-      <c r="B30" s="119"/>
-      <c r="C30" s="83" t="s">
+      <c r="B33" s="119"/>
+      <c r="C33" s="83" t="s">
         <v>608</v>
       </c>
-      <c r="D30" s="146"/>
-    </row>
-    <row r="31" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A31" s="119"/>
-      <c r="B31" s="119"/>
-      <c r="C31" s="83" t="s">
+      <c r="D33" s="146"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="119"/>
+      <c r="B34" s="119"/>
+      <c r="C34" s="83" t="s">
         <v>609</v>
       </c>
-      <c r="D31" s="146"/>
-    </row>
-    <row r="32" spans="1:172" x14ac:dyDescent="0.3">
-      <c r="A32" s="139" t="s">
+      <c r="D34" s="146"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="139" t="s">
         <v>210</v>
       </c>
-      <c r="B32" s="140"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="146"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="124" t="s">
+      <c r="B35" s="140"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="146"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="124" t="s">
         <v>610</v>
       </c>
-      <c r="B33" s="124"/>
-      <c r="C33" s="82" t="s">
+      <c r="B36" s="124"/>
+      <c r="C36" s="82" t="s">
         <v>615</v>
       </c>
-      <c r="D33" s="146"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="124"/>
-      <c r="B34" s="124"/>
-      <c r="C34" s="82" t="s">
-        <v>625</v>
-      </c>
-      <c r="D34" s="146"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="119" t="s">
-        <v>611</v>
-      </c>
-      <c r="B35" s="119"/>
-      <c r="C35" s="83" t="s">
-        <v>612</v>
-      </c>
-      <c r="D35" s="146"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="119"/>
-      <c r="B36" s="119"/>
-      <c r="C36" s="83" t="s">
-        <v>613</v>
-      </c>
       <c r="D36" s="146"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="124" t="s">
-        <v>614</v>
-      </c>
+      <c r="A37" s="124"/>
       <c r="B37" s="124"/>
       <c r="C37" s="82" t="s">
-        <v>192</v>
+        <v>625</v>
       </c>
       <c r="D37" s="146"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="124"/>
-      <c r="B38" s="124"/>
-      <c r="C38" s="82" t="s">
-        <v>190</v>
+      <c r="A38" s="119" t="s">
+        <v>611</v>
+      </c>
+      <c r="B38" s="119"/>
+      <c r="C38" s="83" t="s">
+        <v>612</v>
       </c>
       <c r="D38" s="146"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="119" t="s">
-        <v>621</v>
-      </c>
+      <c r="A39" s="119"/>
       <c r="B39" s="119"/>
       <c r="C39" s="83" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D39" s="146"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="119"/>
-      <c r="B40" s="119"/>
-      <c r="C40" s="83" t="s">
-        <v>617</v>
+      <c r="A40" s="124" t="s">
+        <v>614</v>
+      </c>
+      <c r="B40" s="124"/>
+      <c r="C40" s="82" t="s">
+        <v>192</v>
       </c>
       <c r="D40" s="146"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="124" t="s">
-        <v>619</v>
-      </c>
+      <c r="A41" s="124"/>
       <c r="B41" s="124"/>
       <c r="C41" s="82" t="s">
-        <v>622</v>
+        <v>190</v>
       </c>
       <c r="D41" s="146"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="124"/>
-      <c r="B42" s="124"/>
-      <c r="C42" s="82" t="s">
-        <v>623</v>
+      <c r="A42" s="119" t="s">
+        <v>621</v>
+      </c>
+      <c r="B42" s="119"/>
+      <c r="C42" s="83" t="s">
+        <v>616</v>
       </c>
       <c r="D42" s="146"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="124"/>
-      <c r="B43" s="124"/>
-      <c r="C43" s="82" t="s">
-        <v>624</v>
+      <c r="A43" s="119"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="83" t="s">
+        <v>617</v>
       </c>
       <c r="D43" s="146"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="124"/>
+      <c r="A44" s="124" t="s">
+        <v>619</v>
+      </c>
       <c r="B44" s="124"/>
       <c r="C44" s="82" t="s">
+        <v>622</v>
+      </c>
+      <c r="D44" s="146"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="124"/>
+      <c r="B45" s="124"/>
+      <c r="C45" s="82" t="s">
+        <v>623</v>
+      </c>
+      <c r="D45" s="146"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="124"/>
+      <c r="B46" s="124"/>
+      <c r="C46" s="82" t="s">
+        <v>624</v>
+      </c>
+      <c r="D46" s="146"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="124"/>
+      <c r="B47" s="124"/>
+      <c r="C47" s="82" t="s">
         <v>620</v>
       </c>
-      <c r="D44" s="146"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="119" t="s">
+      <c r="D47" s="146"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="119" t="s">
         <v>626</v>
       </c>
-      <c r="B45" s="119"/>
-      <c r="C45" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="146"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="119"/>
-      <c r="B46" s="119"/>
-      <c r="C46" s="83" t="s">
-        <v>627</v>
-      </c>
-      <c r="D46" s="146"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="119"/>
-      <c r="B47" s="119"/>
-      <c r="C47" s="83" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="146"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="119"/>
       <c r="B48" s="119"/>
       <c r="C48" s="83" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D48" s="146"/>
     </row>
@@ -7494,7 +8256,7 @@
       <c r="A49" s="119"/>
       <c r="B49" s="119"/>
       <c r="C49" s="83" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D49" s="146"/>
     </row>
@@ -7502,85 +8264,85 @@
       <c r="A50" s="119"/>
       <c r="B50" s="119"/>
       <c r="C50" s="83" t="s">
-        <v>628</v>
+        <v>66</v>
       </c>
       <c r="D50" s="146"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="119"/>
       <c r="B51" s="119"/>
-      <c r="C51" s="97" t="s">
+      <c r="C51" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" s="146"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="119"/>
+      <c r="B52" s="119"/>
+      <c r="C52" s="83" t="s">
+        <v>630</v>
+      </c>
+      <c r="D52" s="146"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="119"/>
+      <c r="B53" s="119"/>
+      <c r="C53" s="83" t="s">
+        <v>628</v>
+      </c>
+      <c r="D53" s="146"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="119"/>
+      <c r="B54" s="119"/>
+      <c r="C54" s="97" t="s">
         <v>629</v>
       </c>
-      <c r="D51" s="146"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="124" t="s">
+      <c r="D54" s="146"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="124" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="128"/>
-      <c r="C52" s="82" t="s">
+      <c r="B55" s="128"/>
+      <c r="C55" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="D52" s="122" t="s">
+      <c r="D55" s="122" t="s">
         <v>627</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="124"/>
-      <c r="B53" s="128"/>
-      <c r="C53" s="82" t="s">
-        <v>148</v>
-      </c>
-      <c r="D53" s="122"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="124"/>
-      <c r="B54" s="128"/>
-      <c r="C54" s="82" t="s">
-        <v>149</v>
-      </c>
-      <c r="D54" s="122"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="124"/>
-      <c r="B55" s="128"/>
-      <c r="C55" s="83" t="s">
-        <v>636</v>
-      </c>
-      <c r="D55" s="123" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="124"/>
       <c r="B56" s="128"/>
-      <c r="C56" s="83" t="s">
-        <v>143</v>
-      </c>
-      <c r="D56" s="123"/>
+      <c r="C56" s="82" t="s">
+        <v>148</v>
+      </c>
+      <c r="D56" s="122"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="124"/>
       <c r="B57" s="128"/>
-      <c r="C57" s="83" t="s">
-        <v>141</v>
-      </c>
-      <c r="D57" s="123"/>
+      <c r="C57" s="82" t="s">
+        <v>149</v>
+      </c>
+      <c r="D57" s="122"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="124"/>
       <c r="B58" s="128"/>
       <c r="C58" s="83" t="s">
-        <v>144</v>
-      </c>
-      <c r="D58" s="123"/>
+        <v>636</v>
+      </c>
+      <c r="D58" s="123" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="124"/>
       <c r="B59" s="128"/>
       <c r="C59" s="83" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D59" s="123"/>
     </row>
@@ -7588,687 +8350,722 @@
       <c r="A60" s="124"/>
       <c r="B60" s="128"/>
       <c r="C60" s="83" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D60" s="123"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="124"/>
       <c r="B61" s="128"/>
-      <c r="C61" s="82" t="s">
-        <v>335</v>
-      </c>
-      <c r="D61" s="98" t="s">
-        <v>66</v>
-      </c>
+      <c r="C61" s="83" t="s">
+        <v>144</v>
+      </c>
+      <c r="D61" s="123"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="124"/>
       <c r="B62" s="128"/>
       <c r="C62" s="83" t="s">
-        <v>637</v>
-      </c>
-      <c r="D62" s="129" t="s">
-        <v>630</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D62" s="123"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="124"/>
       <c r="B63" s="128"/>
       <c r="C63" s="83" t="s">
-        <v>638</v>
-      </c>
-      <c r="D63" s="130"/>
+        <v>146</v>
+      </c>
+      <c r="D63" s="123"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="124"/>
       <c r="B64" s="128"/>
       <c r="C64" s="82" t="s">
-        <v>589</v>
-      </c>
-      <c r="D64" s="134" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+      <c r="D64" s="98" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="124"/>
       <c r="B65" s="128"/>
-      <c r="C65" s="82" t="s">
-        <v>590</v>
-      </c>
-      <c r="D65" s="137"/>
-    </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="C65" s="83" t="s">
+        <v>637</v>
+      </c>
+      <c r="D65" s="129" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="124"/>
       <c r="B66" s="128"/>
-      <c r="C66" s="82" t="s">
-        <v>591</v>
-      </c>
-      <c r="D66" s="137"/>
-    </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="C66" s="83" t="s">
+        <v>638</v>
+      </c>
+      <c r="D66" s="130"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="124"/>
       <c r="B67" s="128"/>
       <c r="C67" s="82" t="s">
-        <v>592</v>
-      </c>
-      <c r="D67" s="137"/>
-    </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.3">
+        <v>589</v>
+      </c>
+      <c r="D67" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="124"/>
       <c r="B68" s="128"/>
       <c r="C68" s="82" t="s">
-        <v>639</v>
+        <v>590</v>
       </c>
       <c r="D68" s="137"/>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="124"/>
       <c r="B69" s="128"/>
       <c r="C69" s="82" t="s">
-        <v>594</v>
-      </c>
-      <c r="D69" s="133"/>
-    </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.3">
+        <v>591</v>
+      </c>
+      <c r="D69" s="137"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="124"/>
       <c r="B70" s="128"/>
-      <c r="C70" s="83" t="s">
+      <c r="C70" s="82" t="s">
+        <v>592</v>
+      </c>
+      <c r="D70" s="137"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="124"/>
+      <c r="B71" s="128"/>
+      <c r="C71" s="82" t="s">
+        <v>639</v>
+      </c>
+      <c r="D71" s="137"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="124"/>
+      <c r="B72" s="128"/>
+      <c r="C72" s="82" t="s">
+        <v>594</v>
+      </c>
+      <c r="D72" s="133"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="124"/>
+      <c r="B73" s="128"/>
+      <c r="C73" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="D70" s="83" t="s">
+      <c r="D73" s="83" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A71" s="138" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="138" t="s">
         <v>634</v>
       </c>
-      <c r="B71" s="138"/>
-      <c r="C71" s="100" t="s">
+      <c r="B74" s="138"/>
+      <c r="C74" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="D71" s="135" t="s">
+      <c r="D74" s="135" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A72" s="138"/>
-      <c r="B72" s="138"/>
-      <c r="C72" s="101" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="138"/>
+      <c r="B75" s="138"/>
+      <c r="C75" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="D72" s="136"/>
-    </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A73" s="122" t="s">
+      <c r="D75" s="136"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="122" t="s">
         <v>633</v>
       </c>
-      <c r="B73" s="122"/>
-      <c r="C73" s="82" t="s">
+      <c r="B76" s="122"/>
+      <c r="C76" s="82" t="s">
         <v>632</v>
       </c>
-      <c r="D73" s="122" t="s">
+      <c r="D76" s="122" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A74" s="122"/>
-      <c r="B74" s="122"/>
-      <c r="C74" s="82" t="s">
-        <v>221</v>
-      </c>
-      <c r="D74" s="122"/>
-    </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A75" s="123" t="s">
-        <v>635</v>
-      </c>
-      <c r="B75" s="123"/>
-      <c r="C75" s="83" t="s">
-        <v>616</v>
-      </c>
-      <c r="D75" s="123" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A76" s="123"/>
-      <c r="B76" s="123"/>
-      <c r="C76" s="83" t="s">
-        <v>617</v>
-      </c>
-      <c r="D76" s="123"/>
-    </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A77" s="122" t="s">
-        <v>640</v>
-      </c>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="122"/>
       <c r="B77" s="122"/>
       <c r="C77" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="D77" s="122"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="123" t="s">
+        <v>635</v>
+      </c>
+      <c r="B78" s="123"/>
+      <c r="C78" s="83" t="s">
+        <v>616</v>
+      </c>
+      <c r="D78" s="123" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="123"/>
+      <c r="B79" s="123"/>
+      <c r="C79" s="83" t="s">
+        <v>617</v>
+      </c>
+      <c r="D79" s="123"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="122" t="s">
+        <v>640</v>
+      </c>
+      <c r="B80" s="122"/>
+      <c r="C80" s="82" t="s">
         <v>641</v>
       </c>
-      <c r="D77" s="122" t="s">
+      <c r="D80" s="122" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A78" s="122"/>
-      <c r="B78" s="122"/>
-      <c r="C78" s="82" t="s">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A81" s="122"/>
+      <c r="B81" s="122"/>
+      <c r="C81" s="82" t="s">
         <v>642</v>
       </c>
-      <c r="D78" s="122"/>
-    </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A79" s="122"/>
-      <c r="B79" s="122"/>
-      <c r="C79" s="82" t="s">
+      <c r="D81" s="122"/>
+    </row>
+    <row r="82" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A82" s="122"/>
+      <c r="B82" s="122"/>
+      <c r="C82" s="82" t="s">
         <v>643</v>
       </c>
-      <c r="D79" s="122"/>
-      <c r="W79"/>
-      <c r="AE79" s="37"/>
-      <c r="AF79" s="37"/>
-      <c r="AG79"/>
-    </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A80" s="123" t="s">
-        <v>646</v>
-      </c>
-      <c r="B80" s="123"/>
-      <c r="C80" s="103" t="s">
-        <v>293</v>
-      </c>
-      <c r="D80" s="129" t="s">
-        <v>629</v>
-      </c>
-      <c r="W80"/>
-      <c r="AE80" s="37"/>
-      <c r="AF80" s="37"/>
-      <c r="AG80"/>
-    </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A81" s="123"/>
-      <c r="B81" s="123"/>
-      <c r="C81" s="83" t="s">
-        <v>294</v>
-      </c>
-      <c r="D81" s="130"/>
-    </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A82" s="133" t="s">
-        <v>647</v>
-      </c>
-      <c r="B82" s="133"/>
-      <c r="C82" s="112" t="s">
-        <v>194</v>
-      </c>
-      <c r="D82" s="131"/>
+      <c r="D82" s="122"/>
       <c r="W82"/>
       <c r="AE82" s="37"/>
       <c r="AF82" s="37"/>
       <c r="AG82"/>
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A83" s="134"/>
-      <c r="B83" s="134"/>
-      <c r="C83" s="111" t="s">
-        <v>195</v>
-      </c>
-      <c r="D83" s="132"/>
+      <c r="A83" s="123" t="s">
+        <v>646</v>
+      </c>
+      <c r="B83" s="123"/>
+      <c r="C83" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="D83" s="129" t="s">
+        <v>629</v>
+      </c>
+      <c r="W83"/>
+      <c r="AE83" s="37"/>
+      <c r="AF83" s="37"/>
+      <c r="AG83"/>
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A84" s="123" t="s">
-        <v>648</v>
-      </c>
+      <c r="A84" s="123"/>
       <c r="B84" s="123"/>
       <c r="C84" s="83" t="s">
-        <v>657</v>
-      </c>
-      <c r="D84" s="123" t="s">
-        <v>67</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="D84" s="130"/>
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A85" s="123"/>
-      <c r="B85" s="123"/>
-      <c r="C85" s="83" t="s">
-        <v>656</v>
-      </c>
-      <c r="D85" s="123"/>
+      <c r="A85" s="133" t="s">
+        <v>647</v>
+      </c>
+      <c r="B85" s="133"/>
+      <c r="C85" s="112" t="s">
+        <v>194</v>
+      </c>
+      <c r="D85" s="131"/>
+      <c r="W85"/>
+      <c r="AE85" s="37"/>
+      <c r="AF85" s="37"/>
+      <c r="AG85"/>
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A86" s="123" t="s">
-        <v>650</v>
-      </c>
-      <c r="B86" s="123"/>
-      <c r="C86" s="83" t="s">
-        <v>651</v>
-      </c>
-      <c r="D86" s="123"/>
+      <c r="A86" s="134"/>
+      <c r="B86" s="134"/>
+      <c r="C86" s="111" t="s">
+        <v>195</v>
+      </c>
+      <c r="D86" s="132"/>
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A87" s="123"/>
+      <c r="A87" s="123" t="s">
+        <v>648</v>
+      </c>
       <c r="B87" s="123"/>
       <c r="C87" s="83" t="s">
-        <v>652</v>
-      </c>
-      <c r="D87" s="123"/>
+        <v>657</v>
+      </c>
+      <c r="D87" s="123" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A88" s="123" t="s">
-        <v>653</v>
-      </c>
+      <c r="A88" s="123"/>
       <c r="B88" s="123"/>
       <c r="C88" s="83" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="D88" s="123"/>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A89" s="123"/>
+      <c r="A89" s="123" t="s">
+        <v>650</v>
+      </c>
       <c r="B89" s="123"/>
       <c r="C89" s="83" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D89" s="123"/>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A90" s="122" t="s">
-        <v>659</v>
-      </c>
-      <c r="B90" s="122"/>
-      <c r="C90" s="82" t="s">
-        <v>645</v>
-      </c>
+      <c r="A90" s="123"/>
+      <c r="B90" s="123"/>
+      <c r="C90" s="83" t="s">
+        <v>652</v>
+      </c>
+      <c r="D90" s="123"/>
     </row>
     <row r="91" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A91" s="122"/>
-      <c r="B91" s="122"/>
-      <c r="C91" s="82" t="s">
-        <v>649</v>
-      </c>
+      <c r="A91" s="123" t="s">
+        <v>653</v>
+      </c>
+      <c r="B91" s="123"/>
+      <c r="C91" s="83" t="s">
+        <v>654</v>
+      </c>
+      <c r="D91" s="123"/>
     </row>
     <row r="92" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A92" s="123" t="s">
-        <v>660</v>
-      </c>
+      <c r="A92" s="123"/>
       <c r="B92" s="123"/>
       <c r="C92" s="83" t="s">
+        <v>655</v>
+      </c>
+      <c r="D92" s="123"/>
+    </row>
+    <row r="93" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A93" s="122" t="s">
+        <v>659</v>
+      </c>
+      <c r="B93" s="122"/>
+      <c r="C93" s="82" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="94" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A94" s="122"/>
+      <c r="B94" s="122"/>
+      <c r="C94" s="82" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="95" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A95" s="123" t="s">
+        <v>660</v>
+      </c>
+      <c r="B95" s="123"/>
+      <c r="C95" s="83" t="s">
         <v>662</v>
       </c>
-      <c r="AB92" s="9"/>
-    </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A93" s="123"/>
-      <c r="B93" s="123"/>
-      <c r="C93" s="83" t="s">
+      <c r="AB95" s="9"/>
+    </row>
+    <row r="96" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A96" s="123"/>
+      <c r="B96" s="123"/>
+      <c r="C96" s="83" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A94" s="129"/>
-      <c r="B94" s="129"/>
-      <c r="C94" s="97" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="129"/>
+      <c r="B97" s="129"/>
+      <c r="C97" s="97" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A95" s="122" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="122" t="s">
         <v>664</v>
       </c>
-      <c r="B95" s="122"/>
-      <c r="C95" s="82" t="s">
+      <c r="B98" s="122"/>
+      <c r="C98" s="82" t="s">
         <v>665</v>
       </c>
-      <c r="D95" s="122" t="s">
+      <c r="D98" s="122" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A96" s="122"/>
-      <c r="B96" s="122"/>
-      <c r="C96" s="82" t="s">
-        <v>666</v>
-      </c>
-      <c r="D96" s="122"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="123" t="s">
-        <v>667</v>
-      </c>
-      <c r="B97" s="123"/>
-      <c r="C97" s="83" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="123"/>
-      <c r="B98" s="123"/>
-      <c r="C98" s="83" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="122" t="s">
-        <v>668</v>
-      </c>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="122"/>
       <c r="B99" s="122"/>
       <c r="C99" s="82" t="s">
+        <v>666</v>
+      </c>
+      <c r="D99" s="122"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="123" t="s">
+        <v>667</v>
+      </c>
+      <c r="B100" s="123"/>
+      <c r="C100" s="83" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="122"/>
-      <c r="B100" s="122"/>
-      <c r="C100" s="82" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="123" t="s">
-        <v>669</v>
-      </c>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="123"/>
       <c r="B101" s="123"/>
       <c r="C101" s="83" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="122" t="s">
+        <v>668</v>
+      </c>
+      <c r="B102" s="122"/>
+      <c r="C102" s="82" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="123"/>
-      <c r="B102" s="123"/>
-      <c r="C102" s="83" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="122"/>
+      <c r="B103" s="122"/>
+      <c r="C103" s="82" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="124" t="s">
-        <v>670</v>
-      </c>
-      <c r="B103" s="128"/>
-      <c r="C103" s="114" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="123" t="s">
+        <v>669</v>
+      </c>
+      <c r="B104" s="123"/>
+      <c r="C104" s="83" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="124"/>
-      <c r="B104" s="128"/>
-      <c r="C104" s="111" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="123" t="s">
-        <v>672</v>
-      </c>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="123"/>
       <c r="B105" s="123"/>
       <c r="C105" s="83" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="124" t="s">
+        <v>670</v>
+      </c>
+      <c r="B106" s="128"/>
+      <c r="C106" s="114" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="123"/>
-      <c r="B106" s="123"/>
-      <c r="C106" s="83" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="124"/>
+      <c r="B107" s="128"/>
+      <c r="C107" s="111" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="122" t="s">
-        <v>671</v>
-      </c>
-      <c r="B107" s="122"/>
-      <c r="C107" s="82" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="123" t="s">
+        <v>672</v>
+      </c>
+      <c r="B108" s="123"/>
+      <c r="C108" s="83" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="122"/>
-      <c r="B108" s="122"/>
-      <c r="C108" s="82" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="123" t="s">
-        <v>673</v>
-      </c>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="123"/>
       <c r="B109" s="123"/>
       <c r="C109" s="83" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="122" t="s">
+        <v>671</v>
+      </c>
+      <c r="B110" s="122"/>
+      <c r="C110" s="82" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="123"/>
-      <c r="B110" s="123"/>
-      <c r="C110" s="83" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="122" t="s">
-        <v>674</v>
-      </c>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="122"/>
       <c r="B111" s="122"/>
       <c r="C111" s="82" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="122"/>
-      <c r="B112" s="122"/>
-      <c r="C112" s="82" t="s">
-        <v>685</v>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="123" t="s">
+        <v>673</v>
+      </c>
+      <c r="B112" s="123"/>
+      <c r="C112" s="83" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="123" t="s">
-        <v>675</v>
-      </c>
+      <c r="A113" s="123"/>
       <c r="B113" s="123"/>
       <c r="C113" s="83" t="s">
-        <v>632</v>
-      </c>
-      <c r="D113" s="83" t="s">
-        <v>676</v>
+        <v>221</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="123"/>
-      <c r="B114" s="123"/>
-      <c r="C114" s="83" t="s">
-        <v>221</v>
-      </c>
-      <c r="D114" s="83"/>
+      <c r="A114" s="122" t="s">
+        <v>674</v>
+      </c>
+      <c r="B114" s="122"/>
+      <c r="C114" s="82" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="122" t="s">
-        <v>677</v>
-      </c>
+      <c r="A115" s="122"/>
       <c r="B115" s="122"/>
       <c r="C115" s="82" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="123" t="s">
+        <v>675</v>
+      </c>
+      <c r="B116" s="123"/>
+      <c r="C116" s="83" t="s">
+        <v>632</v>
+      </c>
+      <c r="D116" s="83" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="123"/>
+      <c r="B117" s="123"/>
+      <c r="C117" s="83" t="s">
+        <v>221</v>
+      </c>
+      <c r="D117" s="83"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="122" t="s">
+        <v>677</v>
+      </c>
+      <c r="B118" s="122"/>
+      <c r="C118" s="82" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="122"/>
-      <c r="B116" s="122"/>
-      <c r="C116" s="82" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="122"/>
+      <c r="B119" s="122"/>
+      <c r="C119" s="82" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="122"/>
-      <c r="B117" s="122"/>
-      <c r="C117" s="82" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="125" t="s">
-        <v>678</v>
-      </c>
-      <c r="B118" s="118"/>
-      <c r="C118" s="83" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="126"/>
-      <c r="B119" s="127"/>
-      <c r="C119" s="83" t="s">
-        <v>221</v>
-      </c>
-    </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="122" t="s">
-        <v>679</v>
-      </c>
+      <c r="A120" s="122"/>
       <c r="B120" s="122"/>
       <c r="C120" s="82" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="125" t="s">
+        <v>678</v>
+      </c>
+      <c r="B121" s="118"/>
+      <c r="C121" s="83" t="s">
         <v>632</v>
       </c>
-      <c r="D120" s="124" t="s">
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="126"/>
+      <c r="B122" s="127"/>
+      <c r="C122" s="83" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="122" t="s">
+        <v>679</v>
+      </c>
+      <c r="B123" s="122"/>
+      <c r="C123" s="82" t="s">
+        <v>632</v>
+      </c>
+      <c r="D123" s="124" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="122"/>
-      <c r="B121" s="122"/>
-      <c r="C121" s="82" t="s">
-        <v>221</v>
-      </c>
-      <c r="D121" s="124"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="123" t="s">
-        <v>680</v>
-      </c>
-      <c r="B122" s="123"/>
-      <c r="C122" s="83" t="s">
-        <v>632</v>
-      </c>
-      <c r="D122" s="124"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="123"/>
-      <c r="B123" s="123"/>
-      <c r="C123" s="83" t="s">
-        <v>221</v>
-      </c>
-      <c r="D123" s="124"/>
-    </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="122" t="s">
-        <v>681</v>
-      </c>
+      <c r="A124" s="122"/>
       <c r="B124" s="122"/>
       <c r="C124" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="D124" s="124"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="123" t="s">
+        <v>680</v>
+      </c>
+      <c r="B125" s="123"/>
+      <c r="C125" s="83" t="s">
         <v>632</v>
       </c>
-      <c r="D124" s="124"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="122"/>
-      <c r="B125" s="122"/>
-      <c r="C125" s="82" t="s">
+      <c r="D125" s="124"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="123"/>
+      <c r="B126" s="123"/>
+      <c r="C126" s="83" t="s">
         <v>221</v>
       </c>
-      <c r="D125" s="124"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="117" t="s">
-        <v>684</v>
-      </c>
-      <c r="B126" s="118"/>
-      <c r="C126" s="83" t="s">
+      <c r="D126" s="124"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="122" t="s">
+        <v>681</v>
+      </c>
+      <c r="B127" s="122"/>
+      <c r="C127" s="82" t="s">
         <v>632</v>
       </c>
-      <c r="D126" s="121" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="119"/>
-      <c r="B127" s="120"/>
-      <c r="C127" s="97" t="s">
-        <v>221</v>
-      </c>
-      <c r="D127" s="121"/>
+      <c r="D127" s="124"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="122" t="s">
-        <v>682</v>
-      </c>
+      <c r="A128" s="122"/>
       <c r="B128" s="122"/>
       <c r="C128" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="D128" s="124"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="117" t="s">
+        <v>684</v>
+      </c>
+      <c r="B129" s="118"/>
+      <c r="C129" s="83" t="s">
+        <v>632</v>
+      </c>
+      <c r="D129" s="121" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="119"/>
+      <c r="B130" s="120"/>
+      <c r="C130" s="97" t="s">
+        <v>221</v>
+      </c>
+      <c r="D130" s="121"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="122" t="s">
+        <v>682</v>
+      </c>
+      <c r="B131" s="122"/>
+      <c r="C131" s="82" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="122"/>
-      <c r="B129" s="122"/>
-      <c r="C129" s="82" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="122"/>
+      <c r="B132" s="122"/>
+      <c r="C132" s="82" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="122"/>
-      <c r="B130" s="122"/>
-      <c r="C130" s="82" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="122"/>
+      <c r="B133" s="122"/>
+      <c r="C133" s="82" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" s="123" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="123" t="s">
         <v>683</v>
       </c>
-      <c r="B131" s="123"/>
-      <c r="C131" s="83" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" s="123"/>
-      <c r="B132" s="123"/>
-      <c r="C132" s="83" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" s="123"/>
-      <c r="B133" s="123"/>
-      <c r="C133" s="83" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" s="123"/>
       <c r="B134" s="123"/>
       <c r="C134" s="83" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="123"/>
       <c r="B135" s="123"/>
       <c r="C135" s="83" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="123"/>
+      <c r="B136" s="123"/>
+      <c r="C136" s="83" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="123"/>
+      <c r="B137" s="123"/>
+      <c r="C137" s="83" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="129"/>
+      <c r="B138" s="129"/>
+      <c r="C138" s="97" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="155" spans="29:33" x14ac:dyDescent="0.3">
-      <c r="AC155" s="28"/>
-      <c r="AG155"/>
-    </row>
-    <row r="156" spans="29:33" x14ac:dyDescent="0.3">
-      <c r="AC156" s="28"/>
-    </row>
-    <row r="157" spans="29:33" x14ac:dyDescent="0.3">
-      <c r="AC157" s="28"/>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="146" t="s">
+        <v>694</v>
+      </c>
+      <c r="B139" s="146"/>
+      <c r="C139" s="148" t="s">
+        <v>632</v>
+      </c>
+      <c r="D139" s="146" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="146"/>
+      <c r="B140" s="146"/>
+      <c r="C140" s="148" t="s">
+        <v>221</v>
+      </c>
+      <c r="D140" s="146"/>
     </row>
     <row r="158" spans="29:33" x14ac:dyDescent="0.3">
       <c r="AC158" s="28"/>
+      <c r="AG158"/>
     </row>
     <row r="159" spans="29:33" x14ac:dyDescent="0.3">
       <c r="AC159" s="28"/>
@@ -8306,94 +9103,109 @@
     <row r="170" spans="29:32" x14ac:dyDescent="0.3">
       <c r="AC170" s="28"/>
     </row>
+    <row r="171" spans="29:32" x14ac:dyDescent="0.3">
+      <c r="AC171" s="28"/>
+    </row>
+    <row r="172" spans="29:32" x14ac:dyDescent="0.3">
+      <c r="AC172" s="28"/>
+    </row>
     <row r="173" spans="29:32" x14ac:dyDescent="0.3">
-      <c r="AE173" s="40"/>
-      <c r="AF173" s="40"/>
+      <c r="AC173" s="28"/>
+    </row>
+    <row r="176" spans="29:32" x14ac:dyDescent="0.3">
+      <c r="AE176" s="40"/>
+      <c r="AF176" s="40"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:FS153" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}"/>
-  <mergeCells count="59">
-    <mergeCell ref="A99:B100"/>
-    <mergeCell ref="A90:B91"/>
-    <mergeCell ref="A92:B94"/>
-    <mergeCell ref="A95:B96"/>
-    <mergeCell ref="D95:D96"/>
-    <mergeCell ref="A97:B98"/>
-    <mergeCell ref="A77:B79"/>
-    <mergeCell ref="D77:D79"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="A26:B27"/>
-    <mergeCell ref="D22:D51"/>
-    <mergeCell ref="A45:B51"/>
-    <mergeCell ref="A39:B40"/>
-    <mergeCell ref="A41:B44"/>
-    <mergeCell ref="A75:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="A30:B31"/>
+  <autoFilter ref="A1:FS156" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}"/>
+  <mergeCells count="61">
+    <mergeCell ref="A139:B140"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="A102:B103"/>
+    <mergeCell ref="A93:B94"/>
+    <mergeCell ref="A95:B97"/>
+    <mergeCell ref="A98:B99"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="A100:B101"/>
+    <mergeCell ref="A80:B82"/>
+    <mergeCell ref="D80:D82"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="A29:B30"/>
+    <mergeCell ref="D25:D54"/>
+    <mergeCell ref="A48:B54"/>
+    <mergeCell ref="A42:B43"/>
+    <mergeCell ref="A44:B47"/>
+    <mergeCell ref="A78:B79"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="A31:B32"/>
     <mergeCell ref="A33:B34"/>
-    <mergeCell ref="A35:B36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="A71:B72"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A73:B74"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="D64:D69"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A52:B70"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="D55:D60"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="D84:D89"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="A80:B81"/>
-    <mergeCell ref="A82:B83"/>
-    <mergeCell ref="A84:B85"/>
-    <mergeCell ref="A86:B87"/>
-    <mergeCell ref="A88:B89"/>
-    <mergeCell ref="A101:B102"/>
-    <mergeCell ref="A103:B104"/>
-    <mergeCell ref="A105:B106"/>
-    <mergeCell ref="A107:B108"/>
-    <mergeCell ref="A109:B110"/>
-    <mergeCell ref="A111:B112"/>
-    <mergeCell ref="A113:B114"/>
-    <mergeCell ref="A115:B117"/>
-    <mergeCell ref="A118:B119"/>
-    <mergeCell ref="A120:B121"/>
-    <mergeCell ref="A126:B127"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="A128:B130"/>
-    <mergeCell ref="A131:B135"/>
-    <mergeCell ref="A122:B123"/>
-    <mergeCell ref="A124:B125"/>
-    <mergeCell ref="D120:D125"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="A74:B75"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A76:B77"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="D67:D72"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A55:B73"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="D58:D63"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="D87:D92"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="A83:B84"/>
+    <mergeCell ref="A85:B86"/>
+    <mergeCell ref="A87:B88"/>
+    <mergeCell ref="A89:B90"/>
+    <mergeCell ref="A91:B92"/>
+    <mergeCell ref="A104:B105"/>
+    <mergeCell ref="A106:B107"/>
+    <mergeCell ref="A108:B109"/>
+    <mergeCell ref="A110:B111"/>
+    <mergeCell ref="A112:B113"/>
+    <mergeCell ref="A114:B115"/>
+    <mergeCell ref="A116:B117"/>
+    <mergeCell ref="A118:B120"/>
+    <mergeCell ref="A121:B122"/>
+    <mergeCell ref="A123:B124"/>
+    <mergeCell ref="A129:B130"/>
+    <mergeCell ref="D129:D130"/>
+    <mergeCell ref="A131:B133"/>
+    <mergeCell ref="A134:B138"/>
+    <mergeCell ref="A125:B126"/>
+    <mergeCell ref="A127:B128"/>
+    <mergeCell ref="D123:D128"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F4197077-37C4-4505-ABA9-5A694BB3C346}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{5C4818FE-8F28-4E23-B374-FB906B5FB666}"/>
-    <hyperlink ref="C12" r:id="rId3" xr:uid="{56F73CAD-B3D0-46AD-9F59-AB50EDA51FF7}"/>
-    <hyperlink ref="C14" r:id="rId4" xr:uid="{FF6E8A38-10E4-4A34-8CB4-3E905E7D33A7}"/>
-    <hyperlink ref="C16" r:id="rId5" xr:uid="{F9106E2D-69EE-417D-B02F-C628D0CBE51E}"/>
-    <hyperlink ref="C15" r:id="rId6" xr:uid="{5D2E6952-6DCB-4CEA-8FAA-D0D7A9B045C5}"/>
-    <hyperlink ref="C17" r:id="rId7" xr:uid="{BE38C964-B449-4477-8524-1C0B16BC140F}"/>
-    <hyperlink ref="C18" r:id="rId8" xr:uid="{E8614FF7-B294-42F2-A654-22E1F43B0F80}"/>
-    <hyperlink ref="C8:C10" r:id="rId9" display="test.gpe+32@outlook.fr" xr:uid="{D163FE48-D705-4EB1-9A48-82364747C5C6}"/>
-    <hyperlink ref="C10" r:id="rId10" xr:uid="{1E07095B-385A-497E-96A2-607EB2A77829}"/>
-    <hyperlink ref="C8" r:id="rId11" xr:uid="{BC070589-401A-4B18-B15A-5B759CC5DD86}"/>
-    <hyperlink ref="C5" r:id="rId12" xr:uid="{751892D5-00C7-4D8D-881E-8A007FCD5FB9}"/>
-    <hyperlink ref="C13" r:id="rId13" xr:uid="{F90A0876-BE67-43B0-9F92-5AA5FA687F8D}"/>
-    <hyperlink ref="C3" r:id="rId14" xr:uid="{A67AD39C-DE35-456E-A0B9-16F23679CB74}"/>
-    <hyperlink ref="C4" r:id="rId15" xr:uid="{644DC2C3-754F-4CB6-9E7B-D46B3B117263}"/>
-    <hyperlink ref="C6" r:id="rId16" xr:uid="{4584FAEB-A325-4126-ADBC-7912949A5763}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{5C4818FE-8F28-4E23-B374-FB906B5FB666}"/>
+    <hyperlink ref="C15" r:id="rId3" xr:uid="{56F73CAD-B3D0-46AD-9F59-AB50EDA51FF7}"/>
+    <hyperlink ref="C17" r:id="rId4" xr:uid="{FF6E8A38-10E4-4A34-8CB4-3E905E7D33A7}"/>
+    <hyperlink ref="C19" r:id="rId5" xr:uid="{F9106E2D-69EE-417D-B02F-C628D0CBE51E}"/>
+    <hyperlink ref="C18" r:id="rId6" xr:uid="{5D2E6952-6DCB-4CEA-8FAA-D0D7A9B045C5}"/>
+    <hyperlink ref="C20" r:id="rId7" xr:uid="{BE38C964-B449-4477-8524-1C0B16BC140F}"/>
+    <hyperlink ref="C21" r:id="rId8" xr:uid="{E8614FF7-B294-42F2-A654-22E1F43B0F80}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{BC070589-401A-4B18-B15A-5B759CC5DD86}"/>
+    <hyperlink ref="C5" r:id="rId10" xr:uid="{751892D5-00C7-4D8D-881E-8A007FCD5FB9}"/>
+    <hyperlink ref="C16" r:id="rId11" xr:uid="{F90A0876-BE67-43B0-9F92-5AA5FA687F8D}"/>
+    <hyperlink ref="C3" r:id="rId12" xr:uid="{A67AD39C-DE35-456E-A0B9-16F23679CB74}"/>
+    <hyperlink ref="C4" r:id="rId13" xr:uid="{644DC2C3-754F-4CB6-9E7B-D46B3B117263}"/>
+    <hyperlink ref="C6" r:id="rId14" xr:uid="{4584FAEB-A325-4126-ADBC-7912949A5763}"/>
+    <hyperlink ref="C7" r:id="rId15" xr:uid="{11D06ED8-0163-4BD3-B7EC-4FC989E6BF36}"/>
+    <hyperlink ref="C8" r:id="rId16" xr:uid="{9159709B-AE08-4E23-97A6-A07BD3F40F3D}"/>
+    <hyperlink ref="C10" r:id="rId17" xr:uid="{6F259305-E0BB-4705-8504-E9395404BA72}"/>
+    <hyperlink ref="C11" r:id="rId18" xr:uid="{D94609D4-7141-4FB9-B555-D7FEF10EBFC5}"/>
+    <hyperlink ref="C12" r:id="rId19" xr:uid="{8B81B9E7-D192-4E51-814A-E019EAD664BD}"/>
+    <hyperlink ref="C14" r:id="rId20" xr:uid="{4559D4CB-5C14-44AA-A0AD-66C252B74A01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
adaptation mesures d'execution IAT
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbenjemi\Katalon Studio\ANEF_Eloignement_V1_Nawres\ANEF-Eloignement\ANEF_Eloignement_V1_Nawres\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D538AB59-496F-41BA-9A81-8FFBEBE6ACF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AE9E46-745D-4FCB-B6E7-9CA60C4A9AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="698">
   <si>
     <t>URL_ANEFdevfenv5</t>
   </si>
@@ -2138,6 +2138,9 @@
   </si>
   <si>
     <t>L. 751-6</t>
+  </si>
+  <si>
+    <t>L. 741-2</t>
   </si>
 </sst>
 </file>
@@ -3364,9 +3367,9 @@
   <dimension ref="A1:FS176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AH1" sqref="AH1"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="L23" activeCellId="1" sqref="L17 L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3720,7 +3723,7 @@
         <v>658</v>
       </c>
       <c r="E2" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F2" s="106">
         <v>7503182091</v>
@@ -3955,7 +3958,7 @@
         <v>658</v>
       </c>
       <c r="E3" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F3" s="106">
         <v>7503182093</v>
@@ -4040,11 +4043,11 @@
       <c r="AL3" s="104"/>
       <c r="AM3" s="104"/>
       <c r="AN3" s="104"/>
-      <c r="AO3" s="11"/>
-      <c r="AP3" s="11"/>
-      <c r="AQ3" s="14"/>
-      <c r="AR3" s="12"/>
-      <c r="AS3" s="11"/>
+      <c r="AO3" s="104"/>
+      <c r="AP3" s="104"/>
+      <c r="AQ3" s="116"/>
+      <c r="AR3" s="147"/>
+      <c r="AS3" s="104"/>
       <c r="AT3" s="28"/>
       <c r="AU3" s="28"/>
       <c r="AV3" s="2"/>
@@ -4182,7 +4185,7 @@
         <v>658</v>
       </c>
       <c r="E4" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F4" s="106">
         <v>7503182109</v>
@@ -4275,11 +4278,11 @@
       <c r="AN4" s="104" t="s">
         <v>632</v>
       </c>
-      <c r="AO4" s="11"/>
-      <c r="AP4" s="11"/>
-      <c r="AQ4" s="14"/>
-      <c r="AR4" s="12"/>
-      <c r="AS4" s="11"/>
+      <c r="AO4" s="104"/>
+      <c r="AP4" s="104"/>
+      <c r="AQ4" s="116"/>
+      <c r="AR4" s="147"/>
+      <c r="AS4" s="104"/>
       <c r="AT4" s="28"/>
       <c r="AU4" s="28"/>
       <c r="AV4" s="2"/>
@@ -4506,11 +4509,11 @@
       <c r="AN5" s="104" t="s">
         <v>632</v>
       </c>
-      <c r="AO5" s="11"/>
-      <c r="AP5" s="11"/>
-      <c r="AQ5" s="14"/>
-      <c r="AR5" s="12"/>
-      <c r="AS5" s="11"/>
+      <c r="AO5" s="104"/>
+      <c r="AP5" s="104"/>
+      <c r="AQ5" s="116"/>
+      <c r="AR5" s="147"/>
+      <c r="AS5" s="104"/>
       <c r="AT5" s="28"/>
       <c r="AU5" s="28"/>
       <c r="AV5" s="2"/>
@@ -4706,17 +4709,17 @@
       <c r="AE6" s="115" t="s">
         <v>221</v>
       </c>
-      <c r="AF6" s="28"/>
+      <c r="AF6" s="115"/>
       <c r="AG6" s="2" t="s">
         <v>632</v>
       </c>
       <c r="AH6" s="104"/>
       <c r="AI6" s="104"/>
-      <c r="AJ6" s="11"/>
-      <c r="AK6" s="11"/>
-      <c r="AL6" s="11"/>
-      <c r="AM6" s="11"/>
-      <c r="AN6" s="11"/>
+      <c r="AJ6" s="104"/>
+      <c r="AK6" s="104"/>
+      <c r="AL6" s="104"/>
+      <c r="AM6" s="104"/>
+      <c r="AN6" s="104"/>
       <c r="AO6" s="104" t="s">
         <v>632</v>
       </c>
@@ -4729,7 +4732,7 @@
       <c r="AR6" s="147" t="s">
         <v>632</v>
       </c>
-      <c r="AS6" s="11"/>
+      <c r="AS6" s="104"/>
       <c r="AT6" s="28"/>
       <c r="AU6" s="28"/>
       <c r="AV6" s="2"/>
@@ -4922,16 +4925,16 @@
       <c r="AB7" s="73"/>
       <c r="AC7" s="28"/>
       <c r="AD7" s="2"/>
-      <c r="AE7" s="28"/>
-      <c r="AF7" s="28"/>
+      <c r="AE7" s="115"/>
+      <c r="AF7" s="115"/>
       <c r="AG7" s="2"/>
-      <c r="AH7" s="11"/>
-      <c r="AI7" s="11"/>
-      <c r="AJ7" s="11"/>
-      <c r="AK7" s="11"/>
-      <c r="AL7" s="11"/>
-      <c r="AM7" s="11"/>
-      <c r="AN7" s="11"/>
+      <c r="AH7" s="104"/>
+      <c r="AI7" s="104"/>
+      <c r="AJ7" s="104"/>
+      <c r="AK7" s="104"/>
+      <c r="AL7" s="104"/>
+      <c r="AM7" s="104"/>
+      <c r="AN7" s="104"/>
       <c r="AO7" s="104" t="s">
         <v>632</v>
       </c>
@@ -4944,7 +4947,7 @@
       <c r="AR7" s="147" t="s">
         <v>632</v>
       </c>
-      <c r="AS7" s="11"/>
+      <c r="AS7" s="104"/>
       <c r="AT7" s="28"/>
       <c r="AU7" s="28"/>
       <c r="AV7" s="2"/>
@@ -5137,11 +5140,11 @@
       <c r="AB8" s="73"/>
       <c r="AC8" s="28"/>
       <c r="AD8" s="2"/>
-      <c r="AE8" s="28"/>
-      <c r="AF8" s="28"/>
+      <c r="AE8" s="115"/>
+      <c r="AF8" s="115"/>
       <c r="AG8" s="2"/>
-      <c r="AH8" s="11"/>
-      <c r="AI8" s="11"/>
+      <c r="AH8" s="104"/>
+      <c r="AI8" s="104"/>
       <c r="AJ8" s="104" t="s">
         <v>632</v>
       </c>
@@ -5169,7 +5172,7 @@
       <c r="AR8" s="147" t="s">
         <v>221</v>
       </c>
-      <c r="AS8" s="11"/>
+      <c r="AS8" s="104"/>
       <c r="AT8" s="28"/>
       <c r="AU8" s="28"/>
       <c r="AV8" s="2"/>
@@ -5358,8 +5361,8 @@
         <v>632</v>
       </c>
       <c r="AD9" s="2"/>
-      <c r="AE9" s="28"/>
-      <c r="AF9" s="28"/>
+      <c r="AE9" s="115"/>
+      <c r="AF9" s="115"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="104" t="s">
         <v>632</v>
@@ -5382,10 +5385,10 @@
       <c r="AN9" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="AO9" s="11"/>
-      <c r="AP9" s="11"/>
-      <c r="AQ9" s="14"/>
-      <c r="AR9" s="12"/>
+      <c r="AO9" s="104"/>
+      <c r="AP9" s="104"/>
+      <c r="AQ9" s="116"/>
+      <c r="AR9" s="147"/>
       <c r="AS9" s="104" t="s">
         <v>632</v>
       </c>
@@ -5577,8 +5580,8 @@
         <v>632</v>
       </c>
       <c r="AD10" s="2"/>
-      <c r="AE10" s="28"/>
-      <c r="AF10" s="28"/>
+      <c r="AE10" s="115"/>
+      <c r="AF10" s="115"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="104" t="s">
         <v>632</v>
@@ -5601,9 +5604,9 @@
       <c r="AN10" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="AO10" s="11"/>
-      <c r="AP10" s="11"/>
-      <c r="AQ10" s="14"/>
+      <c r="AO10" s="104"/>
+      <c r="AP10" s="104"/>
+      <c r="AQ10" s="116"/>
       <c r="AR10" s="147" t="s">
         <v>632</v>
       </c>
@@ -5800,8 +5803,8 @@
         <v>632</v>
       </c>
       <c r="AD11" s="2"/>
-      <c r="AE11" s="28"/>
-      <c r="AF11" s="28"/>
+      <c r="AE11" s="115"/>
+      <c r="AF11" s="115"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="104" t="s">
         <v>632</v>
@@ -5821,14 +5824,14 @@
       <c r="AM11" s="104" t="s">
         <v>308</v>
       </c>
-      <c r="AN11" s="11"/>
-      <c r="AO11" s="11"/>
-      <c r="AP11" s="11"/>
-      <c r="AQ11" s="14"/>
+      <c r="AN11" s="104"/>
+      <c r="AO11" s="104"/>
+      <c r="AP11" s="104"/>
+      <c r="AQ11" s="116"/>
       <c r="AR11" s="147" t="s">
         <v>632</v>
       </c>
-      <c r="AS11" s="11"/>
+      <c r="AS11" s="104"/>
       <c r="AT11" s="28"/>
       <c r="AU11" s="28"/>
       <c r="AV11" s="2"/>
@@ -6019,8 +6022,8 @@
         <v>221</v>
       </c>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="28"/>
-      <c r="AF12" s="28"/>
+      <c r="AE12" s="115"/>
+      <c r="AF12" s="115"/>
       <c r="AG12" s="2" t="s">
         <v>632</v>
       </c>
@@ -6033,17 +6036,17 @@
       <c r="AJ12" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="AK12" s="11"/>
-      <c r="AL12" s="11"/>
-      <c r="AM12" s="11"/>
-      <c r="AN12" s="11"/>
-      <c r="AO12" s="11"/>
-      <c r="AP12" s="11"/>
-      <c r="AQ12" s="14"/>
+      <c r="AK12" s="104"/>
+      <c r="AL12" s="104"/>
+      <c r="AM12" s="104"/>
+      <c r="AN12" s="104"/>
+      <c r="AO12" s="104"/>
+      <c r="AP12" s="104"/>
+      <c r="AQ12" s="116"/>
       <c r="AR12" s="147" t="s">
         <v>632</v>
       </c>
-      <c r="AS12" s="11"/>
+      <c r="AS12" s="104"/>
       <c r="AT12" s="28"/>
       <c r="AU12" s="28"/>
       <c r="AV12" s="2"/>
@@ -6234,34 +6237,35 @@
       <c r="AD13" s="2">
         <v>3</v>
       </c>
-      <c r="AE13" s="28"/>
-      <c r="AF13" s="28"/>
+      <c r="AE13" s="115"/>
+      <c r="AF13" s="115"/>
       <c r="AG13" s="2"/>
-      <c r="AH13" s="11" t="s">
+      <c r="AH13" s="104" t="s">
         <v>632</v>
       </c>
-      <c r="AI13" s="11" t="s">
+      <c r="AI13" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="AJ13" s="11" t="s">
+      <c r="AJ13" s="104" t="s">
         <v>632</v>
       </c>
-      <c r="AK13" s="11" t="s">
+      <c r="AK13" s="104" t="s">
         <v>686</v>
       </c>
-      <c r="AL13" s="11" t="s">
+      <c r="AL13" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="AM13" s="11" t="s">
+      <c r="AM13" s="104" t="s">
         <v>308</v>
       </c>
-      <c r="AN13" s="11" t="s">
+      <c r="AN13" s="104" t="s">
         <v>632</v>
       </c>
-      <c r="AO13" s="11"/>
-      <c r="AP13" s="11"/>
-      <c r="AQ13" s="14"/>
-      <c r="AS13" s="11"/>
+      <c r="AO13" s="104"/>
+      <c r="AP13" s="104"/>
+      <c r="AQ13" s="116"/>
+      <c r="AR13" s="81"/>
+      <c r="AS13" s="104"/>
       <c r="AT13" s="28"/>
       <c r="AU13" s="28"/>
       <c r="AV13" s="2"/>
@@ -6452,37 +6456,37 @@
       <c r="AD14" s="2">
         <v>3</v>
       </c>
-      <c r="AE14" s="28"/>
-      <c r="AF14" s="28"/>
+      <c r="AE14" s="115"/>
+      <c r="AF14" s="115"/>
       <c r="AG14" s="2"/>
-      <c r="AH14" s="11" t="s">
+      <c r="AH14" s="104" t="s">
         <v>632</v>
       </c>
-      <c r="AI14" s="11" t="s">
+      <c r="AI14" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="AJ14" s="11" t="s">
+      <c r="AJ14" s="104" t="s">
         <v>632</v>
       </c>
-      <c r="AK14" s="11" t="s">
+      <c r="AK14" s="104" t="s">
         <v>686</v>
       </c>
-      <c r="AL14" s="11" t="s">
+      <c r="AL14" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="AM14" s="11" t="s">
+      <c r="AM14" s="104" t="s">
         <v>308</v>
       </c>
-      <c r="AN14" s="11" t="s">
+      <c r="AN14" s="104" t="s">
         <v>632</v>
       </c>
-      <c r="AO14" s="11"/>
-      <c r="AP14" s="11"/>
-      <c r="AQ14" s="14"/>
-      <c r="AR14" s="12" t="s">
+      <c r="AO14" s="104"/>
+      <c r="AP14" s="104"/>
+      <c r="AQ14" s="116"/>
+      <c r="AR14" s="147" t="s">
         <v>632</v>
       </c>
-      <c r="AS14" s="11"/>
+      <c r="AS14" s="104"/>
       <c r="AT14" s="28"/>
       <c r="AU14" s="28"/>
       <c r="AV14" s="2"/>
@@ -6620,10 +6624,10 @@
         <v>187</v>
       </c>
       <c r="E15" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F15" s="106">
-        <v>7703056113</v>
+        <v>7503182091</v>
       </c>
       <c r="G15" s="106" t="s">
         <v>615</v>
@@ -6657,29 +6661,51 @@
       <c r="T15" s="84"/>
       <c r="U15" s="84"/>
       <c r="V15" s="84"/>
-      <c r="W15" s="84"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="11"/>
+      <c r="W15" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X15" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y15" s="104" t="s">
+        <v>665</v>
+      </c>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="73"/>
-      <c r="AC15" s="28"/>
+      <c r="AC15" s="115" t="s">
+        <v>221</v>
+      </c>
       <c r="AD15" s="2"/>
-      <c r="AE15" s="28"/>
-      <c r="AF15" s="28"/>
+      <c r="AE15" s="115"/>
+      <c r="AF15" s="115"/>
       <c r="AG15" s="2"/>
-      <c r="AH15" s="11"/>
-      <c r="AI15" s="11"/>
-      <c r="AJ15" s="11"/>
-      <c r="AK15" s="11"/>
-      <c r="AL15" s="11"/>
-      <c r="AM15" s="11"/>
-      <c r="AN15" s="11"/>
-      <c r="AO15" s="11"/>
-      <c r="AP15" s="11"/>
-      <c r="AQ15" s="14"/>
-      <c r="AR15" s="12"/>
-      <c r="AS15" s="11"/>
+      <c r="AH15" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI15" s="104" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ15" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AK15" s="104" t="s">
+        <v>686</v>
+      </c>
+      <c r="AL15" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM15" s="104" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN15" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AO15" s="104"/>
+      <c r="AP15" s="104"/>
+      <c r="AQ15" s="116"/>
+      <c r="AR15" s="147"/>
+      <c r="AS15" s="104"/>
       <c r="AT15" s="28"/>
       <c r="AU15" s="28"/>
       <c r="AV15" s="2"/>
@@ -6817,7 +6843,7 @@
         <v>187</v>
       </c>
       <c r="E16" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F16" s="106">
         <v>7703056113</v>
@@ -6854,29 +6880,55 @@
       <c r="T16" s="84"/>
       <c r="U16" s="84"/>
       <c r="V16" s="84"/>
-      <c r="W16" s="84"/>
-      <c r="X16" s="28"/>
-      <c r="Y16" s="11"/>
+      <c r="W16" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X16" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y16" s="104" t="s">
+        <v>697</v>
+      </c>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="73"/>
-      <c r="AC16" s="28"/>
+      <c r="AC16" s="115" t="s">
+        <v>632</v>
+      </c>
       <c r="AD16" s="2"/>
-      <c r="AE16" s="28"/>
-      <c r="AF16" s="28"/>
+      <c r="AE16" s="115" t="s">
+        <v>632</v>
+      </c>
+      <c r="AF16" s="115" t="s">
+        <v>290</v>
+      </c>
       <c r="AG16" s="2"/>
-      <c r="AH16" s="11"/>
-      <c r="AI16" s="11"/>
-      <c r="AJ16" s="11"/>
-      <c r="AK16" s="11"/>
-      <c r="AL16" s="11"/>
-      <c r="AM16" s="11"/>
-      <c r="AN16" s="11"/>
-      <c r="AO16" s="11"/>
-      <c r="AP16" s="11"/>
-      <c r="AQ16" s="14"/>
-      <c r="AR16" s="12"/>
-      <c r="AS16" s="11"/>
+      <c r="AH16" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="AI16" s="104"/>
+      <c r="AJ16" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AK16" s="104" t="s">
+        <v>686</v>
+      </c>
+      <c r="AL16" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM16" s="104" t="s">
+        <v>309</v>
+      </c>
+      <c r="AN16" s="104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AO16" s="104"/>
+      <c r="AP16" s="104"/>
+      <c r="AQ16" s="116"/>
+      <c r="AR16" s="147" t="s">
+        <v>632</v>
+      </c>
+      <c r="AS16" s="104"/>
       <c r="AT16" s="28"/>
       <c r="AU16" s="28"/>
       <c r="AV16" s="2"/>
@@ -9185,24 +9237,24 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F4197077-37C4-4505-ABA9-5A694BB3C346}"/>
     <hyperlink ref="C13" r:id="rId2" xr:uid="{5C4818FE-8F28-4E23-B374-FB906B5FB666}"/>
-    <hyperlink ref="C15" r:id="rId3" xr:uid="{56F73CAD-B3D0-46AD-9F59-AB50EDA51FF7}"/>
-    <hyperlink ref="C17" r:id="rId4" xr:uid="{FF6E8A38-10E4-4A34-8CB4-3E905E7D33A7}"/>
-    <hyperlink ref="C19" r:id="rId5" xr:uid="{F9106E2D-69EE-417D-B02F-C628D0CBE51E}"/>
-    <hyperlink ref="C18" r:id="rId6" xr:uid="{5D2E6952-6DCB-4CEA-8FAA-D0D7A9B045C5}"/>
-    <hyperlink ref="C20" r:id="rId7" xr:uid="{BE38C964-B449-4477-8524-1C0B16BC140F}"/>
-    <hyperlink ref="C21" r:id="rId8" xr:uid="{E8614FF7-B294-42F2-A654-22E1F43B0F80}"/>
-    <hyperlink ref="C9" r:id="rId9" xr:uid="{BC070589-401A-4B18-B15A-5B759CC5DD86}"/>
-    <hyperlink ref="C5" r:id="rId10" xr:uid="{751892D5-00C7-4D8D-881E-8A007FCD5FB9}"/>
-    <hyperlink ref="C16" r:id="rId11" xr:uid="{F90A0876-BE67-43B0-9F92-5AA5FA687F8D}"/>
-    <hyperlink ref="C3" r:id="rId12" xr:uid="{A67AD39C-DE35-456E-A0B9-16F23679CB74}"/>
-    <hyperlink ref="C4" r:id="rId13" xr:uid="{644DC2C3-754F-4CB6-9E7B-D46B3B117263}"/>
-    <hyperlink ref="C6" r:id="rId14" xr:uid="{4584FAEB-A325-4126-ADBC-7912949A5763}"/>
-    <hyperlink ref="C7" r:id="rId15" xr:uid="{11D06ED8-0163-4BD3-B7EC-4FC989E6BF36}"/>
-    <hyperlink ref="C8" r:id="rId16" xr:uid="{9159709B-AE08-4E23-97A6-A07BD3F40F3D}"/>
-    <hyperlink ref="C10" r:id="rId17" xr:uid="{6F259305-E0BB-4705-8504-E9395404BA72}"/>
-    <hyperlink ref="C11" r:id="rId18" xr:uid="{D94609D4-7141-4FB9-B555-D7FEF10EBFC5}"/>
-    <hyperlink ref="C12" r:id="rId19" xr:uid="{8B81B9E7-D192-4E51-814A-E019EAD664BD}"/>
-    <hyperlink ref="C14" r:id="rId20" xr:uid="{4559D4CB-5C14-44AA-A0AD-66C252B74A01}"/>
+    <hyperlink ref="C17" r:id="rId3" xr:uid="{FF6E8A38-10E4-4A34-8CB4-3E905E7D33A7}"/>
+    <hyperlink ref="C19" r:id="rId4" xr:uid="{F9106E2D-69EE-417D-B02F-C628D0CBE51E}"/>
+    <hyperlink ref="C18" r:id="rId5" xr:uid="{5D2E6952-6DCB-4CEA-8FAA-D0D7A9B045C5}"/>
+    <hyperlink ref="C20" r:id="rId6" xr:uid="{BE38C964-B449-4477-8524-1C0B16BC140F}"/>
+    <hyperlink ref="C21" r:id="rId7" xr:uid="{E8614FF7-B294-42F2-A654-22E1F43B0F80}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{BC070589-401A-4B18-B15A-5B759CC5DD86}"/>
+    <hyperlink ref="C5" r:id="rId9" xr:uid="{751892D5-00C7-4D8D-881E-8A007FCD5FB9}"/>
+    <hyperlink ref="C16" r:id="rId10" xr:uid="{F90A0876-BE67-43B0-9F92-5AA5FA687F8D}"/>
+    <hyperlink ref="C3" r:id="rId11" xr:uid="{A67AD39C-DE35-456E-A0B9-16F23679CB74}"/>
+    <hyperlink ref="C4" r:id="rId12" xr:uid="{644DC2C3-754F-4CB6-9E7B-D46B3B117263}"/>
+    <hyperlink ref="C6" r:id="rId13" xr:uid="{4584FAEB-A325-4126-ADBC-7912949A5763}"/>
+    <hyperlink ref="C7" r:id="rId14" xr:uid="{11D06ED8-0163-4BD3-B7EC-4FC989E6BF36}"/>
+    <hyperlink ref="C8" r:id="rId15" xr:uid="{9159709B-AE08-4E23-97A6-A07BD3F40F3D}"/>
+    <hyperlink ref="C10" r:id="rId16" xr:uid="{6F259305-E0BB-4705-8504-E9395404BA72}"/>
+    <hyperlink ref="C11" r:id="rId17" xr:uid="{D94609D4-7141-4FB9-B555-D7FEF10EBFC5}"/>
+    <hyperlink ref="C12" r:id="rId18" xr:uid="{8B81B9E7-D192-4E51-814A-E019EAD664BD}"/>
+    <hyperlink ref="C14" r:id="rId19" xr:uid="{4559D4CB-5C14-44AA-A0AD-66C252B74A01}"/>
+    <hyperlink ref="C15" r:id="rId20" xr:uid="{71554E80-69BA-48C8-B3FF-E4B8CA18AFED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId21"/>

</xml_diff>

<commit_message>
adaptation mesures d'execution ITF
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbenjemi\Katalon Studio\ANEF_Eloignement_V1_Nawres\ANEF-Eloignement\ANEF_Eloignement_V1_Nawres\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AE9E46-745D-4FCB-B6E7-9CA60C4A9AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3290D93A-617C-43FE-978F-68018123CB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="699">
   <si>
     <t>URL_ANEFdevfenv5</t>
   </si>
@@ -2141,6 +2141,9 @@
   </si>
   <si>
     <t>L. 741-2</t>
+  </si>
+  <si>
+    <t>AjouterRelevement</t>
   </si>
 </sst>
 </file>
@@ -2622,7 +2625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3048,9 +3051,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3366,10 +3366,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}">
   <dimension ref="A1:FS176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AH1" sqref="AH1"/>
-      <selection pane="bottomLeft" activeCell="L23" activeCellId="1" sqref="L17 L23"/>
+      <selection pane="bottomLeft" activeCell="AN16" sqref="AN16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3580,7 +3580,9 @@
       <c r="AS1" s="13" t="s">
         <v>694</v>
       </c>
-      <c r="AT1" s="13"/>
+      <c r="AT1" s="13" t="s">
+        <v>698</v>
+      </c>
       <c r="AU1" s="13"/>
       <c r="AV1" s="23"/>
       <c r="AW1" s="23"/>
@@ -6264,7 +6266,7 @@
       <c r="AO13" s="104"/>
       <c r="AP13" s="104"/>
       <c r="AQ13" s="116"/>
-      <c r="AR13" s="81"/>
+      <c r="AR13" s="147"/>
       <c r="AS13" s="104"/>
       <c r="AT13" s="28"/>
       <c r="AU13" s="28"/>
@@ -6920,7 +6922,7 @@
         <v>309</v>
       </c>
       <c r="AN16" s="104" t="s">
-        <v>632</v>
+        <v>221</v>
       </c>
       <c r="AO16" s="104"/>
       <c r="AP16" s="104"/>
@@ -7057,16 +7059,16 @@
         <v>74</v>
       </c>
       <c r="B17" s="104" t="s">
-        <v>599</v>
+        <v>76</v>
       </c>
       <c r="C17" s="105" t="s">
-        <v>644</v>
+        <v>631</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>658</v>
+        <v>187</v>
       </c>
       <c r="E17" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F17" s="106">
         <v>7503182086</v>
@@ -7107,16 +7109,28 @@
       <c r="V17" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="W17" s="84"/>
-      <c r="X17" s="28"/>
-      <c r="Y17" s="11"/>
+      <c r="W17" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X17" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y17" s="104" t="s">
+        <v>665</v>
+      </c>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="73"/>
-      <c r="AC17" s="28"/>
+      <c r="AC17" s="115" t="s">
+        <v>632</v>
+      </c>
       <c r="AD17" s="2"/>
-      <c r="AE17" s="28"/>
-      <c r="AF17" s="28"/>
+      <c r="AE17" s="115" t="s">
+        <v>632</v>
+      </c>
+      <c r="AF17" s="115" t="s">
+        <v>291</v>
+      </c>
       <c r="AG17" s="2"/>
       <c r="AH17" s="11"/>
       <c r="AI17" s="11"/>
@@ -7308,20 +7322,38 @@
       <c r="V18" s="84" t="s">
         <v>655</v>
       </c>
-      <c r="W18" s="84"/>
-      <c r="X18" s="28"/>
-      <c r="Y18" s="11"/>
+      <c r="W18" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X18" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y18" s="104" t="s">
+        <v>665</v>
+      </c>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
+      <c r="AA18" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB18" s="73"/>
-      <c r="AC18" s="28"/>
+      <c r="AC18" s="28" t="s">
+        <v>221</v>
+      </c>
       <c r="AD18" s="2"/>
-      <c r="AE18" s="28"/>
+      <c r="AE18" s="28" t="s">
+        <v>221</v>
+      </c>
       <c r="AF18" s="28"/>
       <c r="AG18" s="2"/>
-      <c r="AH18" s="11"/>
-      <c r="AI18" s="11"/>
-      <c r="AJ18" s="11"/>
+      <c r="AH18" s="11" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI18" s="11" t="s">
+        <v>666</v>
+      </c>
+      <c r="AJ18" s="11" t="s">
+        <v>221</v>
+      </c>
       <c r="AK18" s="11"/>
       <c r="AL18" s="11"/>
       <c r="AM18" s="11"/>
@@ -7331,7 +7363,9 @@
       <c r="AQ18" s="14"/>
       <c r="AR18" s="12"/>
       <c r="AS18" s="11"/>
-      <c r="AT18" s="28"/>
+      <c r="AT18" s="28" t="s">
+        <v>632</v>
+      </c>
       <c r="AU18" s="28"/>
       <c r="AV18" s="2"/>
       <c r="AW18" s="2"/>
@@ -7507,20 +7541,36 @@
       <c r="V19" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="W19" s="84"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="11"/>
+      <c r="W19" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X19" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y19" s="104" t="s">
+        <v>665</v>
+      </c>
       <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
+      <c r="AA19" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="AB19" s="73"/>
       <c r="AC19" s="28"/>
       <c r="AD19" s="2"/>
-      <c r="AE19" s="28"/>
+      <c r="AE19" s="28" t="s">
+        <v>221</v>
+      </c>
       <c r="AF19" s="28"/>
       <c r="AG19" s="2"/>
-      <c r="AH19" s="11"/>
-      <c r="AI19" s="11"/>
-      <c r="AJ19" s="11"/>
+      <c r="AH19" s="11" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI19" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ19" s="11" t="s">
+        <v>221</v>
+      </c>
       <c r="AK19" s="11"/>
       <c r="AL19" s="11"/>
       <c r="AM19" s="11"/>
@@ -7528,7 +7578,9 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
       <c r="AQ19" s="14"/>
-      <c r="AR19" s="12"/>
+      <c r="AR19" s="147" t="s">
+        <v>221</v>
+      </c>
       <c r="AS19" s="11"/>
       <c r="AT19" s="28"/>
       <c r="AU19" s="28"/>
@@ -7667,7 +7719,7 @@
         <v>187</v>
       </c>
       <c r="E20" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F20" s="106">
         <v>7703056113</v>
@@ -7706,9 +7758,15 @@
       <c r="V20" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="W20" s="84"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="11"/>
+      <c r="W20" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="X20" s="113" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y20" s="104" t="s">
+        <v>697</v>
+      </c>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="73"/>
@@ -7866,7 +7924,7 @@
         <v>187</v>
       </c>
       <c r="E21" s="106" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F21" s="106">
         <v>7703056113</v>
@@ -7905,7 +7963,9 @@
       <c r="V21" s="84" t="s">
         <v>654</v>
       </c>
-      <c r="W21" s="84"/>
+      <c r="W21" s="84" t="s">
+        <v>649</v>
+      </c>
       <c r="X21" s="28"/>
       <c r="Y21" s="11"/>
       <c r="Z21" s="1"/>
@@ -9096,24 +9156,44 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" s="146" t="s">
+      <c r="A139" s="122" t="s">
         <v>694</v>
       </c>
-      <c r="B139" s="146"/>
-      <c r="C139" s="148" t="s">
+      <c r="B139" s="122"/>
+      <c r="C139" s="82" t="s">
         <v>632</v>
       </c>
-      <c r="D139" s="146" t="s">
+      <c r="D139" s="122" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" s="146"/>
-      <c r="B140" s="146"/>
-      <c r="C140" s="148" t="s">
+      <c r="A140" s="122"/>
+      <c r="B140" s="122"/>
+      <c r="C140" s="82" t="s">
         <v>221</v>
       </c>
-      <c r="D140" s="146"/>
+      <c r="D140" s="122"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="123" t="s">
+        <v>698</v>
+      </c>
+      <c r="B141" s="123"/>
+      <c r="C141" s="83" t="s">
+        <v>632</v>
+      </c>
+      <c r="D141" s="123" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="123"/>
+      <c r="B142" s="123"/>
+      <c r="C142" s="83" t="s">
+        <v>221</v>
+      </c>
+      <c r="D142" s="123"/>
     </row>
     <row r="158" spans="29:33" x14ac:dyDescent="0.3">
       <c r="AC158" s="28"/>
@@ -9170,9 +9250,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:FS156" xr:uid="{E5C91BAD-9DDB-4FBC-A6EC-B86632F6D8AF}"/>
-  <mergeCells count="61">
+  <mergeCells count="63">
     <mergeCell ref="A139:B140"/>
     <mergeCell ref="D139:D140"/>
+    <mergeCell ref="A141:B142"/>
+    <mergeCell ref="D141:D142"/>
     <mergeCell ref="A102:B103"/>
     <mergeCell ref="A93:B94"/>
     <mergeCell ref="A95:B97"/>
@@ -9237,24 +9319,24 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F4197077-37C4-4505-ABA9-5A694BB3C346}"/>
     <hyperlink ref="C13" r:id="rId2" xr:uid="{5C4818FE-8F28-4E23-B374-FB906B5FB666}"/>
-    <hyperlink ref="C17" r:id="rId3" xr:uid="{FF6E8A38-10E4-4A34-8CB4-3E905E7D33A7}"/>
-    <hyperlink ref="C19" r:id="rId4" xr:uid="{F9106E2D-69EE-417D-B02F-C628D0CBE51E}"/>
-    <hyperlink ref="C18" r:id="rId5" xr:uid="{5D2E6952-6DCB-4CEA-8FAA-D0D7A9B045C5}"/>
-    <hyperlink ref="C20" r:id="rId6" xr:uid="{BE38C964-B449-4477-8524-1C0B16BC140F}"/>
-    <hyperlink ref="C21" r:id="rId7" xr:uid="{E8614FF7-B294-42F2-A654-22E1F43B0F80}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{BC070589-401A-4B18-B15A-5B759CC5DD86}"/>
-    <hyperlink ref="C5" r:id="rId9" xr:uid="{751892D5-00C7-4D8D-881E-8A007FCD5FB9}"/>
-    <hyperlink ref="C16" r:id="rId10" xr:uid="{F90A0876-BE67-43B0-9F92-5AA5FA687F8D}"/>
-    <hyperlink ref="C3" r:id="rId11" xr:uid="{A67AD39C-DE35-456E-A0B9-16F23679CB74}"/>
-    <hyperlink ref="C4" r:id="rId12" xr:uid="{644DC2C3-754F-4CB6-9E7B-D46B3B117263}"/>
-    <hyperlink ref="C6" r:id="rId13" xr:uid="{4584FAEB-A325-4126-ADBC-7912949A5763}"/>
-    <hyperlink ref="C7" r:id="rId14" xr:uid="{11D06ED8-0163-4BD3-B7EC-4FC989E6BF36}"/>
-    <hyperlink ref="C8" r:id="rId15" xr:uid="{9159709B-AE08-4E23-97A6-A07BD3F40F3D}"/>
-    <hyperlink ref="C10" r:id="rId16" xr:uid="{6F259305-E0BB-4705-8504-E9395404BA72}"/>
-    <hyperlink ref="C11" r:id="rId17" xr:uid="{D94609D4-7141-4FB9-B555-D7FEF10EBFC5}"/>
-    <hyperlink ref="C12" r:id="rId18" xr:uid="{8B81B9E7-D192-4E51-814A-E019EAD664BD}"/>
-    <hyperlink ref="C14" r:id="rId19" xr:uid="{4559D4CB-5C14-44AA-A0AD-66C252B74A01}"/>
-    <hyperlink ref="C15" r:id="rId20" xr:uid="{71554E80-69BA-48C8-B3FF-E4B8CA18AFED}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{BC070589-401A-4B18-B15A-5B759CC5DD86}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{751892D5-00C7-4D8D-881E-8A007FCD5FB9}"/>
+    <hyperlink ref="C16" r:id="rId5" xr:uid="{F90A0876-BE67-43B0-9F92-5AA5FA687F8D}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{A67AD39C-DE35-456E-A0B9-16F23679CB74}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{644DC2C3-754F-4CB6-9E7B-D46B3B117263}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{4584FAEB-A325-4126-ADBC-7912949A5763}"/>
+    <hyperlink ref="C7" r:id="rId9" xr:uid="{11D06ED8-0163-4BD3-B7EC-4FC989E6BF36}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{9159709B-AE08-4E23-97A6-A07BD3F40F3D}"/>
+    <hyperlink ref="C10" r:id="rId11" xr:uid="{6F259305-E0BB-4705-8504-E9395404BA72}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{D94609D4-7141-4FB9-B555-D7FEF10EBFC5}"/>
+    <hyperlink ref="C12" r:id="rId13" xr:uid="{8B81B9E7-D192-4E51-814A-E019EAD664BD}"/>
+    <hyperlink ref="C14" r:id="rId14" xr:uid="{4559D4CB-5C14-44AA-A0AD-66C252B74A01}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{71554E80-69BA-48C8-B3FF-E4B8CA18AFED}"/>
+    <hyperlink ref="C21" r:id="rId16" xr:uid="{E8614FF7-B294-42F2-A654-22E1F43B0F80}"/>
+    <hyperlink ref="C20" r:id="rId17" xr:uid="{BE38C964-B449-4477-8524-1C0B16BC140F}"/>
+    <hyperlink ref="C18" r:id="rId18" xr:uid="{5D2E6952-6DCB-4CEA-8FAA-D0D7A9B045C5}"/>
+    <hyperlink ref="C19" r:id="rId19" xr:uid="{F9106E2D-69EE-417D-B02F-C628D0CBE51E}"/>
+    <hyperlink ref="C17" r:id="rId20" xr:uid="{BE6EB66F-C87C-4F8F-BC52-5F0829AAA9A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId21"/>

</xml_diff>